<commit_message>
added a row for whether the simulation was with wind or not
</commit_message>
<xml_diff>
--- a/documentation/Phase 2 experiments/Experiments.xlsx
+++ b/documentation/Phase 2 experiments/Experiments.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gebruiker\Documents\Uni\Project 2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\V\Documents\School\Project 2\Github\documentation\Phase 2 experiments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8702DBD-7384-400D-ADE9-2A23447D2F2B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{F6A190E3-661D-4F27-AEC7-3700DE5F73D1}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{715DD086-ACD7-4858-9E34-CEA6F756B20B}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{715DD086-ACD7-4858-9E34-CEA6F756B20B}"/>
   </bookViews>
   <sheets>
     <sheet name="Open Loop" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="19">
   <si>
     <t>x</t>
   </si>
@@ -82,6 +82,12 @@
   </si>
   <si>
     <t>Landing Position (m)</t>
+  </si>
+  <si>
+    <t>With wind ?</t>
+  </si>
+  <si>
+    <t>No</t>
   </si>
 </sst>
 </file>
@@ -196,15 +202,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
@@ -220,6 +217,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -537,8 +543,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCCFA795-07D1-4DA6-81B9-DD5CB576DC0E}">
   <dimension ref="C2:T55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -559,12 +565,12 @@
         <v>7</v>
       </c>
       <c r="G2" s="4"/>
-      <c r="H2" s="8" t="s">
+      <c r="H2" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="I2" s="9"/>
-      <c r="J2" s="9"/>
-      <c r="K2" s="10"/>
+      <c r="I2" s="18"/>
+      <c r="J2" s="18"/>
+      <c r="K2" s="20"/>
       <c r="L2" s="6" t="s">
         <v>12</v>
       </c>
@@ -587,7 +593,7 @@
       <c r="G3" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="H3" s="11" t="s">
+      <c r="H3" s="8" t="s">
         <v>11</v>
       </c>
       <c r="I3" s="3" t="s">
@@ -596,7 +602,7 @@
       <c r="J3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="K3" s="12" t="s">
+      <c r="K3" s="9" t="s">
         <v>5</v>
       </c>
       <c r="L3" s="1" t="s">
@@ -625,7 +631,7 @@
       <c r="G4" s="4">
         <v>0</v>
       </c>
-      <c r="H4" s="13">
+      <c r="H4" s="10">
         <v>196</v>
       </c>
       <c r="I4" s="2">
@@ -634,7 +640,7 @@
       <c r="J4" s="2">
         <v>1</v>
       </c>
-      <c r="K4" s="14">
+      <c r="K4" s="11">
         <v>40</v>
       </c>
       <c r="L4">
@@ -663,7 +669,7 @@
       <c r="G5" s="4">
         <v>0</v>
       </c>
-      <c r="H5" s="13"/>
+      <c r="H5" s="10"/>
       <c r="I5" s="7"/>
       <c r="J5" s="7"/>
       <c r="K5" s="4"/>
@@ -693,7 +699,7 @@
       <c r="G6" s="4">
         <v>0</v>
       </c>
-      <c r="H6" s="13"/>
+      <c r="H6" s="10"/>
       <c r="I6" s="7"/>
       <c r="J6" s="7"/>
       <c r="K6" s="4"/>
@@ -723,7 +729,7 @@
       <c r="G7" s="4">
         <v>0</v>
       </c>
-      <c r="H7" s="13"/>
+      <c r="H7" s="10"/>
       <c r="I7" s="7"/>
       <c r="J7" s="7"/>
       <c r="K7" s="4"/>
@@ -739,10 +745,10 @@
       <c r="O7" s="4">
         <v>0</v>
       </c>
-      <c r="Q7" s="16"/>
-      <c r="R7" s="17"/>
-      <c r="S7" s="18"/>
-      <c r="T7" s="18"/>
+      <c r="Q7" s="13"/>
+      <c r="R7" s="14"/>
+      <c r="S7" s="15"/>
+      <c r="T7" s="15"/>
     </row>
     <row r="8" spans="3:20" x14ac:dyDescent="0.3">
       <c r="C8" s="7"/>
@@ -758,7 +764,7 @@
       <c r="G8" s="4">
         <v>0</v>
       </c>
-      <c r="H8" s="13"/>
+      <c r="H8" s="10"/>
       <c r="I8" s="7"/>
       <c r="J8" s="7"/>
       <c r="K8" s="4"/>
@@ -792,7 +798,7 @@
       <c r="G9" s="4">
         <v>0</v>
       </c>
-      <c r="H9" s="13"/>
+      <c r="H9" s="10"/>
       <c r="I9" s="7"/>
       <c r="J9" s="7"/>
       <c r="K9" s="4"/>
@@ -823,7 +829,7 @@
       <c r="G10" s="4">
         <v>0</v>
       </c>
-      <c r="H10" s="13"/>
+      <c r="H10" s="10"/>
       <c r="I10" s="7"/>
       <c r="J10" s="7"/>
       <c r="K10" s="4"/>
@@ -854,7 +860,7 @@
       <c r="G11" s="4">
         <v>0</v>
       </c>
-      <c r="H11" s="13"/>
+      <c r="H11" s="10"/>
       <c r="I11" s="7"/>
       <c r="J11" s="7"/>
       <c r="K11" s="4"/>
@@ -885,7 +891,7 @@
       <c r="G12" s="4">
         <v>0</v>
       </c>
-      <c r="H12" s="13"/>
+      <c r="H12" s="10"/>
       <c r="I12" s="7"/>
       <c r="J12" s="7"/>
       <c r="K12" s="4"/>
@@ -916,7 +922,7 @@
       <c r="G13" s="4">
         <v>0</v>
       </c>
-      <c r="H13" s="13"/>
+      <c r="H13" s="10"/>
       <c r="I13" s="7"/>
       <c r="J13" s="7"/>
       <c r="K13" s="4"/>
@@ -947,7 +953,7 @@
       <c r="G14" s="4">
         <v>0</v>
       </c>
-      <c r="H14" s="13"/>
+      <c r="H14" s="10"/>
       <c r="I14" s="7"/>
       <c r="J14" s="7"/>
       <c r="K14" s="4"/>
@@ -978,7 +984,7 @@
       <c r="G15" s="4">
         <v>0</v>
       </c>
-      <c r="H15" s="13"/>
+      <c r="H15" s="10"/>
       <c r="I15" s="7"/>
       <c r="J15" s="7"/>
       <c r="K15" s="4"/>
@@ -1009,7 +1015,7 @@
       <c r="G16" s="4">
         <v>0</v>
       </c>
-      <c r="H16" s="13"/>
+      <c r="H16" s="10"/>
       <c r="I16" s="7"/>
       <c r="J16" s="7"/>
       <c r="K16" s="4"/>
@@ -1040,7 +1046,7 @@
       <c r="G17" s="4">
         <v>0</v>
       </c>
-      <c r="H17" s="13"/>
+      <c r="H17" s="10"/>
       <c r="I17" s="7"/>
       <c r="J17" s="7"/>
       <c r="K17" s="4"/>
@@ -1071,7 +1077,7 @@
       <c r="G18" s="4">
         <v>0</v>
       </c>
-      <c r="H18" s="13"/>
+      <c r="H18" s="10"/>
       <c r="I18" s="7"/>
       <c r="J18" s="7"/>
       <c r="K18" s="4"/>
@@ -1102,7 +1108,7 @@
       <c r="G19" s="4">
         <v>0</v>
       </c>
-      <c r="H19" s="13"/>
+      <c r="H19" s="10"/>
       <c r="I19" s="7"/>
       <c r="J19" s="7"/>
       <c r="K19" s="4"/>
@@ -1133,7 +1139,7 @@
       <c r="G20" s="4">
         <v>0</v>
       </c>
-      <c r="H20" s="13"/>
+      <c r="H20" s="10"/>
       <c r="I20" s="7"/>
       <c r="J20" s="7"/>
       <c r="K20" s="4"/>
@@ -1164,7 +1170,7 @@
       <c r="G21" s="4">
         <v>0</v>
       </c>
-      <c r="H21" s="13"/>
+      <c r="H21" s="10"/>
       <c r="I21" s="7"/>
       <c r="J21" s="7"/>
       <c r="K21" s="4"/>
@@ -1195,7 +1201,7 @@
       <c r="G22" s="4">
         <v>0</v>
       </c>
-      <c r="H22" s="13"/>
+      <c r="H22" s="10"/>
       <c r="I22" s="7"/>
       <c r="J22" s="7"/>
       <c r="K22" s="4"/>
@@ -1226,7 +1232,7 @@
       <c r="G23" s="4">
         <v>0</v>
       </c>
-      <c r="H23" s="13"/>
+      <c r="H23" s="10"/>
       <c r="I23" s="7"/>
       <c r="J23" s="7"/>
       <c r="K23" s="4"/>
@@ -1257,7 +1263,7 @@
       <c r="G24" s="4">
         <v>0</v>
       </c>
-      <c r="H24" s="13"/>
+      <c r="H24" s="10"/>
       <c r="I24" s="7"/>
       <c r="J24" s="7"/>
       <c r="K24" s="4"/>
@@ -1314,20 +1320,20 @@
       <c r="P31" s="7"/>
     </row>
     <row r="33" spans="4:17" x14ac:dyDescent="0.3">
-      <c r="D33" s="20"/>
+      <c r="D33" s="17"/>
       <c r="E33" s="7"/>
-      <c r="F33" s="20"/>
+      <c r="F33" s="17"/>
       <c r="G33" s="7"/>
-      <c r="H33" s="16"/>
-      <c r="I33" s="9"/>
-      <c r="J33" s="9"/>
-      <c r="K33" s="9"/>
-      <c r="L33" s="9"/>
-      <c r="M33" s="20"/>
+      <c r="H33" s="13"/>
+      <c r="I33" s="18"/>
+      <c r="J33" s="18"/>
+      <c r="K33" s="18"/>
+      <c r="L33" s="18"/>
+      <c r="M33" s="17"/>
       <c r="N33" s="7"/>
-      <c r="O33" s="20"/>
+      <c r="O33" s="17"/>
       <c r="P33" s="7"/>
-      <c r="Q33" s="16"/>
+      <c r="Q33" s="13"/>
     </row>
     <row r="34" spans="4:17" x14ac:dyDescent="0.3">
       <c r="D34" s="7"/>
@@ -1693,21 +1699,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F51CB71-A509-4AC5-AC8E-6056CE32F9C4}">
-  <dimension ref="B2:O24"/>
+  <dimension ref="B2:P24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="5" width="11.21875" customWidth="1"/>
-    <col min="6" max="6" width="13.5546875" customWidth="1"/>
-    <col min="11" max="14" width="11.21875" customWidth="1"/>
-    <col min="15" max="15" width="13.5546875" customWidth="1"/>
+    <col min="6" max="7" width="13.5546875" customWidth="1"/>
+    <col min="12" max="15" width="11.21875" customWidth="1"/>
+    <col min="16" max="16" width="13.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B2" s="6" t="s">
         <v>6</v>
       </c>
@@ -1716,28 +1722,31 @@
         <v>7</v>
       </c>
       <c r="E2" s="4"/>
-      <c r="F2" s="15" t="s">
+      <c r="F2" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="8" t="s">
+      <c r="G2" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="H2" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="H2" s="9"/>
-      <c r="I2" s="9"/>
-      <c r="J2" s="10"/>
-      <c r="K2" s="6" t="s">
+      <c r="I2" s="18"/>
+      <c r="J2" s="18"/>
+      <c r="K2" s="20"/>
+      <c r="L2" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="L2" s="4"/>
-      <c r="M2" s="6" t="s">
+      <c r="M2" s="4"/>
+      <c r="N2" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="N2" s="4"/>
-      <c r="O2" s="15" t="s">
+      <c r="O2" s="4"/>
+      <c r="P2" s="12" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
@@ -1750,38 +1759,39 @@
       <c r="E3" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="F3" s="19" t="s">
+      <c r="F3" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="G3" s="11" t="s">
+      <c r="G3" s="16"/>
+      <c r="H3" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="I3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="I3" s="3" t="s">
+      <c r="J3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="J3" s="12" t="s">
+      <c r="K3" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="K3" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="L3" s="5" t="s">
+      <c r="L3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="M3" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="M3" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="N3" s="5" t="s">
+      <c r="N3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="O3" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="O3" s="19" t="s">
+      <c r="P3" s="16" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B4">
         <v>0</v>
       </c>
@@ -1794,38 +1804,41 @@
       <c r="E4" s="4">
         <v>0</v>
       </c>
-      <c r="F4" s="13">
-        <v>0</v>
-      </c>
-      <c r="G4" s="13">
+      <c r="F4" s="10">
+        <v>0</v>
+      </c>
+      <c r="G4" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="H4" s="10">
         <v>196</v>
       </c>
-      <c r="H4" s="2">
+      <c r="I4" s="2">
         <v>10</v>
       </c>
-      <c r="I4" s="2">
+      <c r="J4" s="2">
         <v>1</v>
       </c>
-      <c r="J4" s="14">
+      <c r="K4" s="11">
         <v>40</v>
       </c>
-      <c r="K4">
-        <v>0</v>
-      </c>
-      <c r="L4" s="4">
-        <v>1200000</v>
-      </c>
-      <c r="M4">
-        <v>0</v>
-      </c>
-      <c r="N4" s="4">
-        <v>0</v>
-      </c>
-      <c r="O4" s="13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="L4">
+        <v>0</v>
+      </c>
+      <c r="M4" s="4">
+        <v>1200000</v>
+      </c>
+      <c r="N4">
+        <v>0</v>
+      </c>
+      <c r="O4" s="4">
+        <v>0</v>
+      </c>
+      <c r="P4" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B5">
         <v>-100</v>
       </c>
@@ -1838,30 +1851,33 @@
       <c r="E5" s="4">
         <v>0</v>
       </c>
-      <c r="F5" s="13">
-        <v>0</v>
-      </c>
-      <c r="G5" s="13"/>
-      <c r="H5" s="7"/>
+      <c r="F5" s="10">
+        <v>0</v>
+      </c>
+      <c r="G5" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="H5" s="10"/>
       <c r="I5" s="7"/>
-      <c r="J5" s="4"/>
-      <c r="K5">
+      <c r="J5" s="7"/>
+      <c r="K5" s="4"/>
+      <c r="L5">
         <v>-100</v>
       </c>
-      <c r="L5" s="4">
-        <v>1200000</v>
-      </c>
-      <c r="M5">
-        <v>0</v>
-      </c>
-      <c r="N5" s="4">
-        <v>0</v>
-      </c>
-      <c r="O5" s="13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="M5" s="4">
+        <v>1200000</v>
+      </c>
+      <c r="N5">
+        <v>0</v>
+      </c>
+      <c r="O5" s="4">
+        <v>0</v>
+      </c>
+      <c r="P5" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B6">
         <v>100</v>
       </c>
@@ -1874,30 +1890,33 @@
       <c r="E6" s="4">
         <v>0</v>
       </c>
-      <c r="F6" s="13">
-        <v>0</v>
-      </c>
-      <c r="G6" s="13"/>
-      <c r="H6" s="7"/>
+      <c r="F6" s="10">
+        <v>0</v>
+      </c>
+      <c r="G6" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="H6" s="10"/>
       <c r="I6" s="7"/>
-      <c r="J6" s="4"/>
-      <c r="K6">
+      <c r="J6" s="7"/>
+      <c r="K6" s="4"/>
+      <c r="L6">
         <v>100</v>
       </c>
-      <c r="L6" s="4">
-        <v>1200000</v>
-      </c>
-      <c r="M6">
-        <v>0</v>
-      </c>
-      <c r="N6" s="4">
-        <v>0</v>
-      </c>
-      <c r="O6" s="13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="M6" s="4">
+        <v>1200000</v>
+      </c>
+      <c r="N6">
+        <v>0</v>
+      </c>
+      <c r="O6" s="4">
+        <v>0</v>
+      </c>
+      <c r="P6" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B7">
         <v>-1000</v>
       </c>
@@ -1910,30 +1929,33 @@
       <c r="E7" s="4">
         <v>0</v>
       </c>
-      <c r="F7" s="13">
-        <v>0</v>
-      </c>
-      <c r="G7" s="13"/>
-      <c r="H7" s="7"/>
+      <c r="F7" s="10">
+        <v>0</v>
+      </c>
+      <c r="G7" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="H7" s="10"/>
       <c r="I7" s="7"/>
-      <c r="J7" s="4"/>
-      <c r="K7">
+      <c r="J7" s="7"/>
+      <c r="K7" s="4"/>
+      <c r="L7">
         <v>-1000</v>
       </c>
-      <c r="L7" s="4">
-        <v>1200000</v>
-      </c>
-      <c r="M7">
-        <v>0</v>
-      </c>
-      <c r="N7" s="4">
-        <v>0</v>
-      </c>
-      <c r="O7" s="13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="M7" s="4">
+        <v>1200000</v>
+      </c>
+      <c r="N7">
+        <v>0</v>
+      </c>
+      <c r="O7" s="4">
+        <v>0</v>
+      </c>
+      <c r="P7" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B8">
         <v>1000</v>
       </c>
@@ -1946,30 +1968,33 @@
       <c r="E8" s="4">
         <v>0</v>
       </c>
-      <c r="F8" s="13">
-        <v>0</v>
-      </c>
-      <c r="G8" s="13"/>
-      <c r="H8" s="7"/>
+      <c r="F8" s="10">
+        <v>0</v>
+      </c>
+      <c r="G8" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="H8" s="10"/>
       <c r="I8" s="7"/>
-      <c r="J8" s="4"/>
-      <c r="K8">
+      <c r="J8" s="7"/>
+      <c r="K8" s="4"/>
+      <c r="L8">
         <v>1000</v>
       </c>
-      <c r="L8" s="4">
-        <v>1200000</v>
-      </c>
-      <c r="M8">
-        <v>0</v>
-      </c>
-      <c r="N8" s="4">
-        <v>0</v>
-      </c>
-      <c r="O8" s="13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="M8" s="4">
+        <v>1200000</v>
+      </c>
+      <c r="N8">
+        <v>0</v>
+      </c>
+      <c r="O8" s="4">
+        <v>0</v>
+      </c>
+      <c r="P8" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B9">
         <v>-10000</v>
       </c>
@@ -1982,30 +2007,33 @@
       <c r="E9" s="4">
         <v>0</v>
       </c>
-      <c r="F9" s="13">
-        <v>0</v>
-      </c>
-      <c r="G9" s="13"/>
-      <c r="H9" s="7"/>
+      <c r="F9" s="10">
+        <v>0</v>
+      </c>
+      <c r="G9" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="H9" s="10"/>
       <c r="I9" s="7"/>
-      <c r="J9" s="4"/>
-      <c r="K9">
+      <c r="J9" s="7"/>
+      <c r="K9" s="4"/>
+      <c r="L9">
         <v>-10000</v>
       </c>
-      <c r="L9" s="4">
-        <v>1200000</v>
-      </c>
-      <c r="M9">
-        <v>0</v>
-      </c>
-      <c r="N9" s="4">
-        <v>0</v>
-      </c>
-      <c r="O9" s="13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="M9" s="4">
+        <v>1200000</v>
+      </c>
+      <c r="N9">
+        <v>0</v>
+      </c>
+      <c r="O9" s="4">
+        <v>0</v>
+      </c>
+      <c r="P9" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B10">
         <v>10000</v>
       </c>
@@ -2018,30 +2046,33 @@
       <c r="E10" s="4">
         <v>0</v>
       </c>
-      <c r="F10" s="13">
-        <v>0</v>
-      </c>
-      <c r="G10" s="13"/>
-      <c r="H10" s="7"/>
+      <c r="F10" s="10">
+        <v>0</v>
+      </c>
+      <c r="G10" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="H10" s="10"/>
       <c r="I10" s="7"/>
-      <c r="J10" s="4"/>
-      <c r="K10">
+      <c r="J10" s="7"/>
+      <c r="K10" s="4"/>
+      <c r="L10">
         <v>10000</v>
       </c>
-      <c r="L10" s="4">
-        <v>1200000</v>
-      </c>
-      <c r="M10">
-        <v>0</v>
-      </c>
-      <c r="N10" s="4">
-        <v>0</v>
-      </c>
-      <c r="O10" s="13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="M10" s="4">
+        <v>1200000</v>
+      </c>
+      <c r="N10">
+        <v>0</v>
+      </c>
+      <c r="O10" s="4">
+        <v>0</v>
+      </c>
+      <c r="P10" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B11">
         <v>0</v>
       </c>
@@ -2054,30 +2085,33 @@
       <c r="E11" s="4">
         <v>0</v>
       </c>
-      <c r="F11" s="13">
-        <v>0</v>
-      </c>
-      <c r="G11" s="13"/>
-      <c r="H11" s="7"/>
+      <c r="F11" s="10">
+        <v>15</v>
+      </c>
+      <c r="G11" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="H11" s="10"/>
       <c r="I11" s="7"/>
-      <c r="J11" s="4"/>
-      <c r="K11">
-        <v>0</v>
-      </c>
-      <c r="L11" s="4">
-        <v>1200000</v>
-      </c>
-      <c r="M11">
-        <v>0</v>
-      </c>
-      <c r="N11" s="4">
-        <v>0</v>
-      </c>
-      <c r="O11" s="13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="J11" s="7"/>
+      <c r="K11" s="4"/>
+      <c r="L11">
+        <v>0</v>
+      </c>
+      <c r="M11" s="4">
+        <v>1200000</v>
+      </c>
+      <c r="N11">
+        <v>0</v>
+      </c>
+      <c r="O11" s="4">
+        <v>0</v>
+      </c>
+      <c r="P11" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B12">
         <v>-100</v>
       </c>
@@ -2090,30 +2124,33 @@
       <c r="E12" s="4">
         <v>0</v>
       </c>
-      <c r="F12" s="13">
-        <v>0</v>
-      </c>
-      <c r="G12" s="13"/>
-      <c r="H12" s="7"/>
+      <c r="F12" s="10">
+        <v>0</v>
+      </c>
+      <c r="G12" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="H12" s="10"/>
       <c r="I12" s="7"/>
-      <c r="J12" s="4"/>
-      <c r="K12">
+      <c r="J12" s="7"/>
+      <c r="K12" s="4"/>
+      <c r="L12">
         <v>-100</v>
       </c>
-      <c r="L12" s="4">
-        <v>1200000</v>
-      </c>
-      <c r="M12">
-        <v>0</v>
-      </c>
-      <c r="N12" s="4">
-        <v>0</v>
-      </c>
-      <c r="O12" s="13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="M12" s="4">
+        <v>1200000</v>
+      </c>
+      <c r="N12">
+        <v>0</v>
+      </c>
+      <c r="O12" s="4">
+        <v>0</v>
+      </c>
+      <c r="P12" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B13">
         <v>100</v>
       </c>
@@ -2126,30 +2163,33 @@
       <c r="E13" s="4">
         <v>0</v>
       </c>
-      <c r="F13" s="13">
-        <v>0</v>
-      </c>
-      <c r="G13" s="13"/>
-      <c r="H13" s="7"/>
+      <c r="F13" s="10">
+        <v>0</v>
+      </c>
+      <c r="G13" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="H13" s="10"/>
       <c r="I13" s="7"/>
-      <c r="J13" s="4"/>
-      <c r="K13">
+      <c r="J13" s="7"/>
+      <c r="K13" s="4"/>
+      <c r="L13">
         <v>100</v>
       </c>
-      <c r="L13" s="4">
-        <v>1200000</v>
-      </c>
-      <c r="M13">
-        <v>0</v>
-      </c>
-      <c r="N13" s="4">
-        <v>0</v>
-      </c>
-      <c r="O13" s="13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="M13" s="4">
+        <v>1200000</v>
+      </c>
+      <c r="N13">
+        <v>0</v>
+      </c>
+      <c r="O13" s="4">
+        <v>0</v>
+      </c>
+      <c r="P13" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B14">
         <v>-1000</v>
       </c>
@@ -2162,30 +2202,33 @@
       <c r="E14" s="4">
         <v>0</v>
       </c>
-      <c r="F14" s="13">
-        <v>0</v>
-      </c>
-      <c r="G14" s="13"/>
-      <c r="H14" s="7"/>
+      <c r="F14" s="10">
+        <v>0</v>
+      </c>
+      <c r="G14" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="H14" s="10"/>
       <c r="I14" s="7"/>
-      <c r="J14" s="4"/>
-      <c r="K14">
+      <c r="J14" s="7"/>
+      <c r="K14" s="4"/>
+      <c r="L14">
         <v>-1000</v>
       </c>
-      <c r="L14" s="4">
-        <v>1200000</v>
-      </c>
-      <c r="M14">
-        <v>0</v>
-      </c>
-      <c r="N14" s="4">
-        <v>0</v>
-      </c>
-      <c r="O14" s="13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="M14" s="4">
+        <v>1200000</v>
+      </c>
+      <c r="N14">
+        <v>0</v>
+      </c>
+      <c r="O14" s="4">
+        <v>0</v>
+      </c>
+      <c r="P14" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B15">
         <v>1000</v>
       </c>
@@ -2198,30 +2241,33 @@
       <c r="E15" s="4">
         <v>0</v>
       </c>
-      <c r="F15" s="13">
-        <v>0</v>
-      </c>
-      <c r="G15" s="13"/>
-      <c r="H15" s="7"/>
+      <c r="F15" s="10">
+        <v>0</v>
+      </c>
+      <c r="G15" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="H15" s="10"/>
       <c r="I15" s="7"/>
-      <c r="J15" s="4"/>
-      <c r="K15">
+      <c r="J15" s="7"/>
+      <c r="K15" s="4"/>
+      <c r="L15">
         <v>1000</v>
       </c>
-      <c r="L15" s="4">
-        <v>1200000</v>
-      </c>
-      <c r="M15">
-        <v>0</v>
-      </c>
-      <c r="N15" s="4">
-        <v>0</v>
-      </c>
-      <c r="O15" s="13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="M15" s="4">
+        <v>1200000</v>
+      </c>
+      <c r="N15">
+        <v>0</v>
+      </c>
+      <c r="O15" s="4">
+        <v>0</v>
+      </c>
+      <c r="P15" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B16">
         <v>-10000</v>
       </c>
@@ -2234,30 +2280,33 @@
       <c r="E16" s="4">
         <v>0</v>
       </c>
-      <c r="F16" s="13">
-        <v>0</v>
-      </c>
-      <c r="G16" s="13"/>
-      <c r="H16" s="7"/>
+      <c r="F16" s="10">
+        <v>0</v>
+      </c>
+      <c r="G16" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="H16" s="10"/>
       <c r="I16" s="7"/>
-      <c r="J16" s="4"/>
-      <c r="K16">
+      <c r="J16" s="7"/>
+      <c r="K16" s="4"/>
+      <c r="L16">
         <v>-10000</v>
       </c>
-      <c r="L16" s="4">
-        <v>1200000</v>
-      </c>
-      <c r="M16">
-        <v>0</v>
-      </c>
-      <c r="N16" s="4">
-        <v>0</v>
-      </c>
-      <c r="O16" s="13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="M16" s="4">
+        <v>1200000</v>
+      </c>
+      <c r="N16">
+        <v>0</v>
+      </c>
+      <c r="O16" s="4">
+        <v>0</v>
+      </c>
+      <c r="P16" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B17">
         <v>10000</v>
       </c>
@@ -2270,30 +2319,33 @@
       <c r="E17" s="4">
         <v>0</v>
       </c>
-      <c r="F17" s="13">
-        <v>0</v>
-      </c>
-      <c r="G17" s="13"/>
-      <c r="H17" s="7"/>
+      <c r="F17" s="10">
+        <v>0</v>
+      </c>
+      <c r="G17" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="H17" s="10"/>
       <c r="I17" s="7"/>
-      <c r="J17" s="4"/>
-      <c r="K17">
+      <c r="J17" s="7"/>
+      <c r="K17" s="4"/>
+      <c r="L17">
         <v>10000</v>
       </c>
-      <c r="L17" s="4">
-        <v>1200000</v>
-      </c>
-      <c r="M17">
-        <v>0</v>
-      </c>
-      <c r="N17" s="4">
-        <v>0</v>
-      </c>
-      <c r="O17" s="13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="M17" s="4">
+        <v>1200000</v>
+      </c>
+      <c r="N17">
+        <v>0</v>
+      </c>
+      <c r="O17" s="4">
+        <v>0</v>
+      </c>
+      <c r="P17" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B18">
         <v>0</v>
       </c>
@@ -2306,30 +2358,33 @@
       <c r="E18" s="4">
         <v>0</v>
       </c>
-      <c r="F18" s="13">
-        <v>0</v>
-      </c>
-      <c r="G18" s="13"/>
-      <c r="H18" s="7"/>
+      <c r="F18" s="10">
+        <v>0</v>
+      </c>
+      <c r="G18" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="H18" s="10"/>
       <c r="I18" s="7"/>
-      <c r="J18" s="4"/>
-      <c r="K18">
-        <v>0</v>
-      </c>
-      <c r="L18" s="4">
-        <v>1200000</v>
-      </c>
-      <c r="M18">
-        <v>0</v>
-      </c>
-      <c r="N18" s="4">
-        <v>0</v>
-      </c>
-      <c r="O18" s="13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="J18" s="7"/>
+      <c r="K18" s="4"/>
+      <c r="L18">
+        <v>0</v>
+      </c>
+      <c r="M18" s="4">
+        <v>1200000</v>
+      </c>
+      <c r="N18">
+        <v>0</v>
+      </c>
+      <c r="O18" s="4">
+        <v>0</v>
+      </c>
+      <c r="P18" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B19">
         <v>-100</v>
       </c>
@@ -2342,30 +2397,33 @@
       <c r="E19" s="4">
         <v>0</v>
       </c>
-      <c r="F19" s="13">
-        <v>0</v>
-      </c>
-      <c r="G19" s="13"/>
-      <c r="H19" s="7"/>
+      <c r="F19" s="10">
+        <v>0</v>
+      </c>
+      <c r="G19" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="H19" s="10"/>
       <c r="I19" s="7"/>
-      <c r="J19" s="4"/>
-      <c r="K19">
+      <c r="J19" s="7"/>
+      <c r="K19" s="4"/>
+      <c r="L19">
         <v>-100</v>
       </c>
-      <c r="L19" s="4">
-        <v>1200000</v>
-      </c>
-      <c r="M19">
-        <v>0</v>
-      </c>
-      <c r="N19" s="4">
-        <v>0</v>
-      </c>
-      <c r="O19" s="13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="M19" s="4">
+        <v>1200000</v>
+      </c>
+      <c r="N19">
+        <v>0</v>
+      </c>
+      <c r="O19" s="4">
+        <v>0</v>
+      </c>
+      <c r="P19" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B20">
         <v>100</v>
       </c>
@@ -2378,30 +2436,33 @@
       <c r="E20" s="4">
         <v>0</v>
       </c>
-      <c r="F20" s="13">
-        <v>0</v>
-      </c>
-      <c r="G20" s="13"/>
-      <c r="H20" s="7"/>
+      <c r="F20" s="10">
+        <v>0</v>
+      </c>
+      <c r="G20" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="H20" s="10"/>
       <c r="I20" s="7"/>
-      <c r="J20" s="4"/>
-      <c r="K20">
+      <c r="J20" s="7"/>
+      <c r="K20" s="4"/>
+      <c r="L20">
         <v>100</v>
       </c>
-      <c r="L20" s="4">
-        <v>1200000</v>
-      </c>
-      <c r="M20">
-        <v>0</v>
-      </c>
-      <c r="N20" s="4">
-        <v>0</v>
-      </c>
-      <c r="O20" s="13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="M20" s="4">
+        <v>1200000</v>
+      </c>
+      <c r="N20">
+        <v>0</v>
+      </c>
+      <c r="O20" s="4">
+        <v>0</v>
+      </c>
+      <c r="P20" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B21">
         <v>-1000</v>
       </c>
@@ -2414,30 +2475,33 @@
       <c r="E21" s="4">
         <v>0</v>
       </c>
-      <c r="F21" s="13">
-        <v>0</v>
-      </c>
-      <c r="G21" s="13"/>
-      <c r="H21" s="7"/>
+      <c r="F21" s="10">
+        <v>0</v>
+      </c>
+      <c r="G21" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="H21" s="10"/>
       <c r="I21" s="7"/>
-      <c r="J21" s="4"/>
-      <c r="K21">
+      <c r="J21" s="7"/>
+      <c r="K21" s="4"/>
+      <c r="L21">
         <v>-1000</v>
       </c>
-      <c r="L21" s="4">
-        <v>1200000</v>
-      </c>
-      <c r="M21">
-        <v>0</v>
-      </c>
-      <c r="N21" s="4">
-        <v>0</v>
-      </c>
-      <c r="O21" s="13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="M21" s="4">
+        <v>1200000</v>
+      </c>
+      <c r="N21">
+        <v>0</v>
+      </c>
+      <c r="O21" s="4">
+        <v>0</v>
+      </c>
+      <c r="P21" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B22">
         <v>1000</v>
       </c>
@@ -2450,30 +2514,33 @@
       <c r="E22" s="4">
         <v>0</v>
       </c>
-      <c r="F22" s="13">
-        <v>0</v>
-      </c>
-      <c r="G22" s="13"/>
-      <c r="H22" s="7"/>
+      <c r="F22" s="10">
+        <v>0</v>
+      </c>
+      <c r="G22" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="H22" s="10"/>
       <c r="I22" s="7"/>
-      <c r="J22" s="4"/>
-      <c r="K22">
+      <c r="J22" s="7"/>
+      <c r="K22" s="4"/>
+      <c r="L22">
         <v>1000</v>
       </c>
-      <c r="L22" s="4">
-        <v>1200000</v>
-      </c>
-      <c r="M22">
-        <v>0</v>
-      </c>
-      <c r="N22" s="4">
-        <v>0</v>
-      </c>
-      <c r="O22" s="13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="M22" s="4">
+        <v>1200000</v>
+      </c>
+      <c r="N22">
+        <v>0</v>
+      </c>
+      <c r="O22" s="4">
+        <v>0</v>
+      </c>
+      <c r="P22" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B23">
         <v>-10000</v>
       </c>
@@ -2486,30 +2553,33 @@
       <c r="E23" s="4">
         <v>0</v>
       </c>
-      <c r="F23" s="13">
-        <v>0</v>
-      </c>
-      <c r="G23" s="13"/>
-      <c r="H23" s="7"/>
+      <c r="F23" s="10">
+        <v>0</v>
+      </c>
+      <c r="G23" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="H23" s="10"/>
       <c r="I23" s="7"/>
-      <c r="J23" s="4"/>
-      <c r="K23">
+      <c r="J23" s="7"/>
+      <c r="K23" s="4"/>
+      <c r="L23">
         <v>-10000</v>
       </c>
-      <c r="L23" s="4">
-        <v>1200000</v>
-      </c>
-      <c r="M23">
-        <v>0</v>
-      </c>
-      <c r="N23" s="4">
-        <v>0</v>
-      </c>
-      <c r="O23" s="13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="M23" s="4">
+        <v>1200000</v>
+      </c>
+      <c r="N23">
+        <v>0</v>
+      </c>
+      <c r="O23" s="4">
+        <v>0</v>
+      </c>
+      <c r="P23" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B24">
         <v>10000</v>
       </c>
@@ -2522,32 +2592,35 @@
       <c r="E24" s="4">
         <v>0</v>
       </c>
-      <c r="F24" s="13">
-        <v>0</v>
-      </c>
-      <c r="G24" s="13"/>
-      <c r="H24" s="7"/>
+      <c r="F24" s="10">
+        <v>0</v>
+      </c>
+      <c r="G24" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="H24" s="10"/>
       <c r="I24" s="7"/>
-      <c r="J24" s="4"/>
-      <c r="K24">
+      <c r="J24" s="7"/>
+      <c r="K24" s="4"/>
+      <c r="L24">
         <v>10000</v>
       </c>
-      <c r="L24" s="4">
-        <v>1200000</v>
-      </c>
-      <c r="M24">
-        <v>0</v>
-      </c>
-      <c r="N24" s="4">
-        <v>0</v>
-      </c>
-      <c r="O24" s="13">
+      <c r="M24" s="4">
+        <v>1200000</v>
+      </c>
+      <c r="N24">
+        <v>0</v>
+      </c>
+      <c r="O24" s="4">
+        <v>0</v>
+      </c>
+      <c r="P24" s="10">
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="G2:J2"/>
+    <mergeCell ref="H2:K2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
integrated Joep's experiments and mine and prepared the way for some additional experiments
</commit_message>
<xml_diff>
--- a/documentation/Phase 2 experiments/Experiments.xlsx
+++ b/documentation/Phase 2 experiments/Experiments.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gebruiker\Documents\Uni\Project 2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\V\Documents\School\Project 2\Github\documentation\Phase 2 experiments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D216AC7-4E37-4F60-883B-C7DE30ABCA95}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{3B604B57-05B1-4DC7-B33C-1511056D5E58}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{715DD086-ACD7-4858-9E34-CEA6F756B20B}"/>
+    <workbookView xWindow="3468" yWindow="0" windowWidth="17280" windowHeight="8964" xr2:uid="{715DD086-ACD7-4858-9E34-CEA6F756B20B}"/>
   </bookViews>
   <sheets>
     <sheet name="Open Loop" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="28">
   <si>
     <t>x</t>
   </si>
@@ -84,6 +84,33 @@
     <t>Landing Position (m)</t>
   </si>
   <si>
+    <t>With wind ?</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>modified angle</t>
+  </si>
+  <si>
+    <t>modified x-position</t>
+  </si>
+  <si>
+    <t>modified y-position</t>
+  </si>
+  <si>
+    <t>modified x-velocity</t>
+  </si>
+  <si>
+    <t>modified y-velocity</t>
+  </si>
+  <si>
+    <t>wind</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
     <t>Different velocities</t>
   </si>
   <si>
@@ -94,6 +121,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.000"/>
+  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -199,7 +229,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -217,18 +247,17 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -238,6 +267,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -554,8 +585,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCCFA795-07D1-4DA6-81B9-DD5CB576DC0E}">
   <dimension ref="B2:T55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -576,12 +607,12 @@
         <v>7</v>
       </c>
       <c r="G2" s="4"/>
-      <c r="H2" s="22" t="s">
+      <c r="H2" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="I2" s="21"/>
-      <c r="J2" s="21"/>
-      <c r="K2" s="23"/>
+      <c r="I2" s="20"/>
+      <c r="J2" s="20"/>
+      <c r="K2" s="22"/>
       <c r="L2" s="6" t="s">
         <v>12</v>
       </c>
@@ -630,8 +661,8 @@
       </c>
     </row>
     <row r="4" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B4" s="20" t="s">
-        <v>17</v>
+      <c r="B4" s="23" t="s">
+        <v>26</v>
       </c>
       <c r="D4">
         <v>0</v>
@@ -783,10 +814,10 @@
       <c r="O7" s="4">
         <v>-10.000999999999999</v>
       </c>
-      <c r="Q7" s="13"/>
-      <c r="R7" s="14"/>
-      <c r="S7" s="15"/>
-      <c r="T7" s="15"/>
+      <c r="Q7" s="17"/>
+      <c r="R7" s="13"/>
+      <c r="S7" s="14"/>
+      <c r="T7" s="14"/>
     </row>
     <row r="8" spans="2:20" x14ac:dyDescent="0.3">
       <c r="C8" s="7"/>
@@ -871,8 +902,8 @@
       <c r="Q9" s="7"/>
     </row>
     <row r="10" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B10" s="20" t="s">
-        <v>18</v>
+      <c r="B10" s="23" t="s">
+        <v>27</v>
       </c>
       <c r="D10">
         <v>0</v>
@@ -886,7 +917,7 @@
       <c r="G10" s="4">
         <v>0</v>
       </c>
-      <c r="H10" s="18">
+      <c r="H10" s="24">
         <v>179</v>
       </c>
       <c r="I10" s="2">
@@ -1214,20 +1245,20 @@
       <c r="P31" s="7"/>
     </row>
     <row r="33" spans="4:17" x14ac:dyDescent="0.3">
-      <c r="D33" s="17"/>
+      <c r="D33" s="16"/>
       <c r="E33" s="7"/>
-      <c r="F33" s="17"/>
+      <c r="F33" s="16"/>
       <c r="G33" s="7"/>
-      <c r="H33" s="13"/>
-      <c r="I33" s="21"/>
-      <c r="J33" s="21"/>
-      <c r="K33" s="21"/>
-      <c r="L33" s="21"/>
-      <c r="M33" s="17"/>
+      <c r="H33" s="17"/>
+      <c r="I33" s="20"/>
+      <c r="J33" s="20"/>
+      <c r="K33" s="20"/>
+      <c r="L33" s="20"/>
+      <c r="M33" s="16"/>
       <c r="N33" s="7"/>
-      <c r="O33" s="17"/>
+      <c r="O33" s="16"/>
       <c r="P33" s="7"/>
-      <c r="Q33" s="13"/>
+      <c r="Q33" s="17"/>
     </row>
     <row r="34" spans="4:17" x14ac:dyDescent="0.3">
       <c r="D34" s="7"/>
@@ -1593,21 +1624,22 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F51CB71-A509-4AC5-AC8E-6056CE32F9C4}">
-  <dimension ref="B2:O24"/>
+  <dimension ref="A2:P31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="1" max="1" width="16.88671875" bestFit="1" customWidth="1"/>
     <col min="2" max="5" width="11.21875" customWidth="1"/>
-    <col min="6" max="6" width="13.5546875" customWidth="1"/>
-    <col min="11" max="14" width="11.21875" customWidth="1"/>
-    <col min="15" max="15" width="13.5546875" customWidth="1"/>
+    <col min="6" max="7" width="13.5546875" customWidth="1"/>
+    <col min="12" max="15" width="11.21875" customWidth="1"/>
+    <col min="16" max="16" width="13.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B2" s="6" t="s">
         <v>6</v>
       </c>
@@ -1619,25 +1651,28 @@
       <c r="F2" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="22" t="s">
+      <c r="G2" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="H2" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="H2" s="21"/>
-      <c r="I2" s="21"/>
-      <c r="J2" s="23"/>
-      <c r="K2" s="6" t="s">
+      <c r="I2" s="20"/>
+      <c r="J2" s="20"/>
+      <c r="K2" s="22"/>
+      <c r="L2" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="L2" s="4"/>
-      <c r="M2" s="6" t="s">
+      <c r="M2" s="4"/>
+      <c r="N2" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="N2" s="4"/>
-      <c r="O2" s="12" t="s">
+      <c r="O2" s="4"/>
+      <c r="P2" s="12" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
@@ -1650,38 +1685,39 @@
       <c r="E3" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="F3" s="16" t="s">
+      <c r="F3" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="G3" s="8" t="s">
+      <c r="G3" s="15"/>
+      <c r="H3" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="I3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="I3" s="3" t="s">
+      <c r="J3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="J3" s="9" t="s">
+      <c r="K3" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="K3" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="L3" s="5" t="s">
+      <c r="L3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="M3" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="M3" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="N3" s="5" t="s">
+      <c r="N3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="O3" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="O3" s="16" t="s">
+      <c r="P3" s="15" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B4">
         <v>0</v>
       </c>
@@ -1697,35 +1733,41 @@
       <c r="F4" s="10">
         <v>0</v>
       </c>
-      <c r="G4" s="10">
-        <v>196</v>
-      </c>
-      <c r="H4" s="2">
-        <v>10</v>
+      <c r="G4" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="H4" s="10">
+        <v>2</v>
       </c>
       <c r="I4" s="2">
-        <v>1</v>
-      </c>
-      <c r="J4" s="11">
-        <v>40</v>
-      </c>
-      <c r="K4">
-        <v>0</v>
-      </c>
-      <c r="L4" s="4">
-        <v>1200000</v>
-      </c>
-      <c r="M4">
-        <v>0</v>
-      </c>
-      <c r="N4" s="4">
-        <v>0</v>
-      </c>
-      <c r="O4" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="2:15" x14ac:dyDescent="0.3">
+        <v>15</v>
+      </c>
+      <c r="J4" s="2">
+        <v>33</v>
+      </c>
+      <c r="K4" s="11">
+        <v>4</v>
+      </c>
+      <c r="L4">
+        <v>0</v>
+      </c>
+      <c r="M4" s="4">
+        <v>-0.10100000000000001</v>
+      </c>
+      <c r="N4">
+        <v>0</v>
+      </c>
+      <c r="O4" s="4">
+        <v>-0.94499999999999995</v>
+      </c>
+      <c r="P4" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>20</v>
+      </c>
       <c r="B5">
         <v>-100</v>
       </c>
@@ -1741,27 +1783,38 @@
       <c r="F5" s="10">
         <v>0</v>
       </c>
-      <c r="G5" s="10"/>
-      <c r="H5" s="7"/>
-      <c r="I5" s="7"/>
-      <c r="J5" s="4"/>
-      <c r="K5">
-        <v>-100</v>
-      </c>
-      <c r="L5" s="4">
-        <v>1200000</v>
-      </c>
-      <c r="M5">
-        <v>0</v>
-      </c>
-      <c r="N5" s="4">
-        <v>0</v>
-      </c>
-      <c r="O5" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="G5" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="H5" s="10">
+        <v>2</v>
+      </c>
+      <c r="I5" s="2">
+        <v>15</v>
+      </c>
+      <c r="J5" s="2">
+        <v>30</v>
+      </c>
+      <c r="K5" s="4">
+        <v>19</v>
+      </c>
+      <c r="L5">
+        <v>3.25</v>
+      </c>
+      <c r="M5" s="4">
+        <v>-1.635</v>
+      </c>
+      <c r="N5">
+        <v>-0.55700000000000005</v>
+      </c>
+      <c r="O5" s="4">
+        <v>-1.4159999999999999</v>
+      </c>
+      <c r="P5" s="10">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B6">
         <v>100</v>
       </c>
@@ -1777,27 +1830,38 @@
       <c r="F6" s="10">
         <v>0</v>
       </c>
-      <c r="G6" s="10"/>
-      <c r="H6" s="7"/>
-      <c r="I6" s="7"/>
-      <c r="J6" s="4"/>
-      <c r="K6">
-        <v>100</v>
-      </c>
-      <c r="L6" s="4">
-        <v>1200000</v>
-      </c>
-      <c r="M6">
-        <v>0</v>
-      </c>
-      <c r="N6" s="4">
-        <v>0</v>
-      </c>
-      <c r="O6" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="G6" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="H6" s="10">
+        <v>2</v>
+      </c>
+      <c r="I6" s="2">
+        <v>15</v>
+      </c>
+      <c r="J6" s="2">
+        <v>30</v>
+      </c>
+      <c r="K6" s="4">
+        <v>1</v>
+      </c>
+      <c r="L6">
+        <v>4.8440000000000003</v>
+      </c>
+      <c r="M6" s="4">
+        <v>-3.73E-2</v>
+      </c>
+      <c r="N6">
+        <v>0.9</v>
+      </c>
+      <c r="O6" s="4">
+        <v>-0.93600000000000005</v>
+      </c>
+      <c r="P6" s="10">
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B7">
         <v>-1000</v>
       </c>
@@ -1813,27 +1877,38 @@
       <c r="F7" s="10">
         <v>0</v>
       </c>
-      <c r="G7" s="10"/>
-      <c r="H7" s="7"/>
-      <c r="I7" s="7"/>
-      <c r="J7" s="4"/>
-      <c r="K7">
-        <v>-1000</v>
-      </c>
-      <c r="L7" s="4">
-        <v>1200000</v>
-      </c>
-      <c r="M7">
-        <v>0</v>
-      </c>
-      <c r="N7" s="4">
-        <v>0</v>
-      </c>
-      <c r="O7" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="G7" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="H7" s="10">
+        <v>2</v>
+      </c>
+      <c r="I7" s="2">
+        <v>15</v>
+      </c>
+      <c r="J7" s="2">
+        <v>30</v>
+      </c>
+      <c r="K7" s="4">
+        <v>17</v>
+      </c>
+      <c r="L7">
+        <v>-3.8479999999999999</v>
+      </c>
+      <c r="M7" s="4">
+        <v>-0.26600000000000001</v>
+      </c>
+      <c r="N7">
+        <v>0.71799999999999997</v>
+      </c>
+      <c r="O7" s="4">
+        <v>-1.0609999999999999</v>
+      </c>
+      <c r="P7" s="10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B8">
         <v>1000</v>
       </c>
@@ -1849,27 +1924,38 @@
       <c r="F8" s="10">
         <v>0</v>
       </c>
-      <c r="G8" s="10"/>
-      <c r="H8" s="7"/>
-      <c r="I8" s="7"/>
-      <c r="J8" s="4"/>
-      <c r="K8">
-        <v>1000</v>
-      </c>
-      <c r="L8" s="4">
-        <v>1200000</v>
-      </c>
-      <c r="M8">
-        <v>0</v>
-      </c>
-      <c r="N8" s="4">
-        <v>0</v>
-      </c>
-      <c r="O8" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="G8" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="H8" s="10">
+        <v>2</v>
+      </c>
+      <c r="I8" s="2">
+        <v>15</v>
+      </c>
+      <c r="J8" s="2">
+        <v>30</v>
+      </c>
+      <c r="K8" s="4">
+        <v>9</v>
+      </c>
+      <c r="L8" s="2">
+        <v>9.6739999999999995</v>
+      </c>
+      <c r="M8" s="4">
+        <v>-0.20300000000000001</v>
+      </c>
+      <c r="N8">
+        <v>-0.81299999999999994</v>
+      </c>
+      <c r="O8" s="4">
+        <v>-1.18</v>
+      </c>
+      <c r="P8" s="10">
+        <v>-7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B9">
         <v>-10000</v>
       </c>
@@ -1885,27 +1971,38 @@
       <c r="F9" s="10">
         <v>0</v>
       </c>
-      <c r="G9" s="10"/>
-      <c r="H9" s="7"/>
-      <c r="I9" s="7"/>
-      <c r="J9" s="4"/>
-      <c r="K9">
-        <v>-10000</v>
-      </c>
-      <c r="L9" s="4">
-        <v>1200000</v>
-      </c>
-      <c r="M9">
-        <v>0</v>
-      </c>
-      <c r="N9" s="4">
-        <v>0</v>
-      </c>
-      <c r="O9" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="G9" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="H9" s="10">
+        <v>2</v>
+      </c>
+      <c r="I9" s="2">
+        <v>15</v>
+      </c>
+      <c r="J9" s="2">
+        <v>29</v>
+      </c>
+      <c r="K9" s="4">
+        <v>29</v>
+      </c>
+      <c r="L9">
+        <v>8.2430000000000003</v>
+      </c>
+      <c r="M9" s="4">
+        <v>-4.6399999999999997E-2</v>
+      </c>
+      <c r="N9">
+        <v>-0.66100000000000003</v>
+      </c>
+      <c r="O9" s="4">
+        <v>-0.52500000000000002</v>
+      </c>
+      <c r="P9" s="10">
+        <v>-6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B10">
         <v>10000</v>
       </c>
@@ -1921,533 +2018,837 @@
       <c r="F10" s="10">
         <v>0</v>
       </c>
-      <c r="G10" s="10"/>
-      <c r="H10" s="7"/>
-      <c r="I10" s="7"/>
-      <c r="J10" s="4"/>
-      <c r="K10">
+      <c r="G10" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="H10" s="10">
+        <v>2</v>
+      </c>
+      <c r="I10" s="2">
+        <v>15</v>
+      </c>
+      <c r="J10" s="2">
+        <v>29</v>
+      </c>
+      <c r="K10" s="4">
+        <v>58</v>
+      </c>
+      <c r="L10">
+        <v>3.0379999999999998</v>
+      </c>
+      <c r="M10" s="4">
+        <v>-0.70399999999999996</v>
+      </c>
+      <c r="N10">
+        <v>-1.0529999999999999</v>
+      </c>
+      <c r="O10" s="4">
+        <v>-0.98499999999999999</v>
+      </c>
+      <c r="P10" s="10">
+        <v>-4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11" s="4">
+        <v>12000</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11" s="4">
+        <v>0</v>
+      </c>
+      <c r="F11" s="10">
+        <v>0</v>
+      </c>
+      <c r="G11" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="H11" s="10"/>
+      <c r="I11" s="7"/>
+      <c r="J11" s="7"/>
+      <c r="K11" s="4"/>
+      <c r="L11">
+        <v>1000</v>
+      </c>
+      <c r="M11" s="4">
+        <v>1200000</v>
+      </c>
+      <c r="N11">
+        <v>0</v>
+      </c>
+      <c r="O11" s="4">
+        <v>0</v>
+      </c>
+      <c r="P11" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="B12">
+        <v>0</v>
+      </c>
+      <c r="C12" s="4">
+        <v>120000</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12" s="4">
+        <v>0</v>
+      </c>
+      <c r="F12" s="10">
+        <v>0</v>
+      </c>
+      <c r="G12" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="H12" s="10"/>
+      <c r="I12" s="7"/>
+      <c r="J12" s="7"/>
+      <c r="K12" s="4"/>
+      <c r="L12">
+        <v>-10000</v>
+      </c>
+      <c r="M12" s="4">
+        <v>1200000</v>
+      </c>
+      <c r="N12">
+        <v>0</v>
+      </c>
+      <c r="O12" s="4">
+        <v>0</v>
+      </c>
+      <c r="P12" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="B13">
+        <v>0</v>
+      </c>
+      <c r="C13" s="19">
+        <v>1200000</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13" s="4">
+        <v>0</v>
+      </c>
+      <c r="F13" s="10">
+        <v>0</v>
+      </c>
+      <c r="G13" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="H13" s="10">
+        <v>2</v>
+      </c>
+      <c r="I13" s="2">
+        <v>15</v>
+      </c>
+      <c r="J13" s="2">
+        <v>33</v>
+      </c>
+      <c r="K13" s="11">
+        <v>4</v>
+      </c>
+      <c r="L13">
+        <v>0</v>
+      </c>
+      <c r="M13" s="4">
+        <v>-0.10100000000000001</v>
+      </c>
+      <c r="N13">
+        <v>0</v>
+      </c>
+      <c r="O13" s="4">
+        <v>-0.94499999999999995</v>
+      </c>
+      <c r="P13" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="B14">
+        <v>0</v>
+      </c>
+      <c r="C14" s="4">
+        <v>12000000</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14" s="4">
+        <v>0</v>
+      </c>
+      <c r="F14" s="10">
+        <v>0</v>
+      </c>
+      <c r="G14" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="H14" s="10"/>
+      <c r="I14" s="7"/>
+      <c r="J14" s="7"/>
+      <c r="K14" s="4"/>
+      <c r="L14">
+        <v>0</v>
+      </c>
+      <c r="M14" s="4">
+        <v>1200000</v>
+      </c>
+      <c r="N14">
+        <v>0</v>
+      </c>
+      <c r="O14" s="4">
+        <v>0</v>
+      </c>
+      <c r="P14" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>19</v>
+      </c>
+      <c r="B15">
+        <v>0</v>
+      </c>
+      <c r="C15" s="4">
+        <v>1200000</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15" s="4">
+        <v>0</v>
+      </c>
+      <c r="F15" s="10">
+        <v>15</v>
+      </c>
+      <c r="G15" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="H15" s="10">
+        <v>2</v>
+      </c>
+      <c r="I15" s="2">
+        <v>15</v>
+      </c>
+      <c r="J15" s="2">
+        <v>29</v>
+      </c>
+      <c r="K15" s="4">
+        <v>57</v>
+      </c>
+      <c r="L15">
+        <v>4.9130000000000003</v>
+      </c>
+      <c r="M15" s="18">
+        <v>-1.66</v>
+      </c>
+      <c r="N15">
+        <v>0.71499999999999997</v>
+      </c>
+      <c r="O15" s="4">
+        <v>-1.429</v>
+      </c>
+      <c r="P15" s="10">
+        <v>-4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="B16">
+        <v>0</v>
+      </c>
+      <c r="C16" s="4">
+        <v>1200000</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16" s="4">
+        <v>0</v>
+      </c>
+      <c r="F16" s="10">
+        <v>30</v>
+      </c>
+      <c r="G16" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="H16" s="10">
+        <v>2</v>
+      </c>
+      <c r="I16" s="2">
+        <v>15</v>
+      </c>
+      <c r="J16" s="2">
+        <v>30</v>
+      </c>
+      <c r="K16" s="4">
+        <v>17</v>
+      </c>
+      <c r="L16">
+        <v>-2.1320000000000001</v>
+      </c>
+      <c r="M16" s="4">
+        <v>-2.13E-4</v>
+      </c>
+      <c r="N16">
+        <v>-0.66900000000000004</v>
+      </c>
+      <c r="O16" s="4">
+        <v>-1.399</v>
+      </c>
+      <c r="P16" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="B17">
+        <v>0</v>
+      </c>
+      <c r="C17" s="4">
+        <v>1200000</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="E17" s="4">
+        <v>0</v>
+      </c>
+      <c r="F17" s="10">
+        <v>45</v>
+      </c>
+      <c r="G17" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="H17" s="10">
+        <v>2</v>
+      </c>
+      <c r="I17" s="2">
+        <v>15</v>
+      </c>
+      <c r="J17" s="2">
+        <v>30</v>
+      </c>
+      <c r="K17" s="4">
+        <v>2</v>
+      </c>
+      <c r="L17">
+        <v>3.1019999999999999</v>
+      </c>
+      <c r="M17" s="4">
+        <v>-0.64700000000000002</v>
+      </c>
+      <c r="N17">
+        <v>1.0329999999999999</v>
+      </c>
+      <c r="O17" s="4">
+        <v>-1.2490000000000001</v>
+      </c>
+      <c r="P17" s="10">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="B18">
+        <v>0</v>
+      </c>
+      <c r="C18" s="4">
+        <v>1200000</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="E18" s="4">
+        <v>0</v>
+      </c>
+      <c r="F18" s="10">
+        <v>60</v>
+      </c>
+      <c r="G18" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="H18" s="10">
+        <v>2</v>
+      </c>
+      <c r="I18" s="2">
+        <v>15</v>
+      </c>
+      <c r="J18" s="2">
+        <v>29</v>
+      </c>
+      <c r="K18" s="4">
+        <v>32</v>
+      </c>
+      <c r="L18">
+        <v>-9.7279999999999998</v>
+      </c>
+      <c r="M18" s="4">
+        <v>-0.53300000000000003</v>
+      </c>
+      <c r="N18">
+        <v>0.71499999999999997</v>
+      </c>
+      <c r="O18" s="4">
+        <v>-1.1040000000000001</v>
+      </c>
+      <c r="P18" s="10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>22</v>
+      </c>
+      <c r="B19">
+        <v>0</v>
+      </c>
+      <c r="C19" s="4">
+        <v>1200000</v>
+      </c>
+      <c r="D19">
+        <v>100</v>
+      </c>
+      <c r="E19" s="4">
+        <v>0</v>
+      </c>
+      <c r="F19" s="10">
+        <v>0</v>
+      </c>
+      <c r="G19" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="H19" s="10"/>
+      <c r="I19" s="7"/>
+      <c r="J19" s="7"/>
+      <c r="K19" s="4"/>
+      <c r="L19">
+        <v>-100</v>
+      </c>
+      <c r="M19" s="4">
+        <v>1200000</v>
+      </c>
+      <c r="N19">
+        <v>0</v>
+      </c>
+      <c r="O19" s="4">
+        <v>0</v>
+      </c>
+      <c r="P19" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="B20">
+        <v>0</v>
+      </c>
+      <c r="C20" s="4">
+        <v>1200000</v>
+      </c>
+      <c r="D20">
+        <v>1000</v>
+      </c>
+      <c r="E20" s="4">
+        <v>0</v>
+      </c>
+      <c r="F20" s="10">
+        <v>0</v>
+      </c>
+      <c r="G20" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="H20" s="10"/>
+      <c r="I20" s="7"/>
+      <c r="J20" s="7"/>
+      <c r="K20" s="4"/>
+      <c r="L20">
+        <v>100</v>
+      </c>
+      <c r="M20" s="4">
+        <v>1200000</v>
+      </c>
+      <c r="N20">
+        <v>0</v>
+      </c>
+      <c r="O20" s="4">
+        <v>0</v>
+      </c>
+      <c r="P20" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="B21">
+        <v>0</v>
+      </c>
+      <c r="C21" s="4">
+        <v>1200000</v>
+      </c>
+      <c r="D21">
+        <v>-100</v>
+      </c>
+      <c r="E21" s="4">
+        <v>0</v>
+      </c>
+      <c r="F21" s="10">
+        <v>0</v>
+      </c>
+      <c r="G21" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="H21" s="10"/>
+      <c r="I21" s="7"/>
+      <c r="J21" s="7"/>
+      <c r="K21" s="4"/>
+      <c r="L21">
+        <v>-1000</v>
+      </c>
+      <c r="M21" s="4">
+        <v>1200000</v>
+      </c>
+      <c r="N21">
+        <v>0</v>
+      </c>
+      <c r="O21" s="4">
+        <v>0</v>
+      </c>
+      <c r="P21" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="B22">
+        <v>0</v>
+      </c>
+      <c r="C22" s="4">
+        <v>1200000</v>
+      </c>
+      <c r="D22">
+        <v>-1000</v>
+      </c>
+      <c r="E22" s="4">
+        <v>0</v>
+      </c>
+      <c r="F22" s="10">
+        <v>0</v>
+      </c>
+      <c r="G22" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="H22" s="10"/>
+      <c r="I22" s="7"/>
+      <c r="J22" s="7"/>
+      <c r="K22" s="4"/>
+      <c r="L22">
+        <v>1000</v>
+      </c>
+      <c r="M22" s="4">
+        <v>1200000</v>
+      </c>
+      <c r="N22">
+        <v>0</v>
+      </c>
+      <c r="O22" s="4">
+        <v>0</v>
+      </c>
+      <c r="P22" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>23</v>
+      </c>
+      <c r="B23">
+        <v>0</v>
+      </c>
+      <c r="C23" s="4">
+        <v>1200000</v>
+      </c>
+      <c r="D23">
+        <v>0</v>
+      </c>
+      <c r="E23" s="4">
+        <v>100</v>
+      </c>
+      <c r="F23" s="10">
+        <v>0</v>
+      </c>
+      <c r="G23" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="H23" s="10"/>
+      <c r="I23" s="7"/>
+      <c r="J23" s="7"/>
+      <c r="K23" s="4"/>
+      <c r="L23">
+        <v>-10000</v>
+      </c>
+      <c r="M23" s="4">
+        <v>1200000</v>
+      </c>
+      <c r="N23">
+        <v>0</v>
+      </c>
+      <c r="O23" s="4">
+        <v>0</v>
+      </c>
+      <c r="P23" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="B24">
+        <v>0</v>
+      </c>
+      <c r="C24" s="4">
+        <v>1200000</v>
+      </c>
+      <c r="D24">
+        <v>0</v>
+      </c>
+      <c r="E24" s="4">
+        <v>1000</v>
+      </c>
+      <c r="F24" s="10">
+        <v>0</v>
+      </c>
+      <c r="G24" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="H24" s="10"/>
+      <c r="I24" s="7"/>
+      <c r="J24" s="7"/>
+      <c r="K24" s="4"/>
+      <c r="L24">
         <v>10000</v>
       </c>
-      <c r="L10" s="4">
-        <v>1200000</v>
-      </c>
-      <c r="M10">
-        <v>0</v>
-      </c>
-      <c r="N10" s="4">
-        <v>0</v>
-      </c>
-      <c r="O10" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B11">
-        <v>0</v>
-      </c>
-      <c r="C11" s="4">
-        <v>1200000</v>
-      </c>
-      <c r="D11">
-        <v>0</v>
-      </c>
-      <c r="E11" s="4">
-        <v>0</v>
-      </c>
-      <c r="F11" s="10">
-        <v>0</v>
-      </c>
-      <c r="G11" s="10"/>
-      <c r="H11" s="7"/>
-      <c r="I11" s="7"/>
-      <c r="J11" s="4"/>
-      <c r="K11">
-        <v>0</v>
-      </c>
-      <c r="L11" s="4">
-        <v>1200000</v>
-      </c>
-      <c r="M11">
-        <v>0</v>
-      </c>
-      <c r="N11" s="4">
-        <v>0</v>
-      </c>
-      <c r="O11" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B12">
+      <c r="M24" s="4">
+        <v>1200000</v>
+      </c>
+      <c r="N24">
+        <v>0</v>
+      </c>
+      <c r="O24" s="4">
+        <v>0</v>
+      </c>
+      <c r="P24" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="B25">
+        <v>0</v>
+      </c>
+      <c r="C25" s="4">
+        <v>1200000</v>
+      </c>
+      <c r="D25">
+        <v>0</v>
+      </c>
+      <c r="E25" s="4">
         <v>-100</v>
       </c>
-      <c r="C12" s="4">
-        <v>1200000</v>
-      </c>
-      <c r="D12">
-        <v>0</v>
-      </c>
-      <c r="E12" s="4">
-        <v>0</v>
-      </c>
-      <c r="F12" s="10">
-        <v>0</v>
-      </c>
-      <c r="G12" s="10"/>
-      <c r="H12" s="7"/>
-      <c r="I12" s="7"/>
-      <c r="J12" s="4"/>
-      <c r="K12">
-        <v>-100</v>
-      </c>
-      <c r="L12" s="4">
-        <v>1200000</v>
-      </c>
-      <c r="M12">
-        <v>0</v>
-      </c>
-      <c r="N12" s="4">
-        <v>0</v>
-      </c>
-      <c r="O12" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B13">
+      <c r="F25" s="10">
+        <v>0</v>
+      </c>
+      <c r="G25" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="H25" s="10"/>
+      <c r="K25" s="4"/>
+      <c r="M25" s="4">
+        <v>1200000</v>
+      </c>
+      <c r="O25" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="B26">
+        <v>0</v>
+      </c>
+      <c r="C26" s="4">
+        <v>1200000</v>
+      </c>
+      <c r="D26">
+        <v>0</v>
+      </c>
+      <c r="E26" s="4">
+        <v>-1000</v>
+      </c>
+      <c r="F26" s="10">
+        <v>0</v>
+      </c>
+      <c r="G26" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="H26" s="10"/>
+      <c r="K26" s="4"/>
+      <c r="M26" s="4">
+        <v>1200000</v>
+      </c>
+      <c r="O26" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>24</v>
+      </c>
+      <c r="B27">
+        <v>0</v>
+      </c>
+      <c r="C27" s="4">
+        <v>1200000</v>
+      </c>
+      <c r="D27">
+        <v>0</v>
+      </c>
+      <c r="E27" s="4">
+        <v>0</v>
+      </c>
+      <c r="F27" s="10">
+        <v>0</v>
+      </c>
+      <c r="G27" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="H27" s="10"/>
+      <c r="K27" s="4"/>
+      <c r="M27" s="4">
+        <v>1200000</v>
+      </c>
+      <c r="O27" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="B28">
         <v>100</v>
       </c>
-      <c r="C13" s="4">
-        <v>1200000</v>
-      </c>
-      <c r="D13">
-        <v>0</v>
-      </c>
-      <c r="E13" s="4">
-        <v>0</v>
-      </c>
-      <c r="F13" s="10">
-        <v>0</v>
-      </c>
-      <c r="G13" s="10"/>
-      <c r="H13" s="7"/>
-      <c r="I13" s="7"/>
-      <c r="J13" s="4"/>
-      <c r="K13">
+      <c r="C28" s="19">
+        <v>1200000</v>
+      </c>
+      <c r="D28">
+        <v>0</v>
+      </c>
+      <c r="E28" s="4">
+        <v>0</v>
+      </c>
+      <c r="F28" s="10">
+        <v>0</v>
+      </c>
+      <c r="G28" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="H28" s="10"/>
+      <c r="K28" s="4"/>
+      <c r="M28" s="4">
+        <v>1200000</v>
+      </c>
+      <c r="O28" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="B29">
+        <v>0</v>
+      </c>
+      <c r="C29" s="19">
+        <v>1200000</v>
+      </c>
+      <c r="D29">
         <v>100</v>
       </c>
-      <c r="L13" s="4">
-        <v>1200000</v>
-      </c>
-      <c r="M13">
-        <v>0</v>
-      </c>
-      <c r="N13" s="4">
-        <v>0</v>
-      </c>
-      <c r="O13" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B14">
-        <v>-1000</v>
-      </c>
-      <c r="C14" s="4">
-        <v>1200000</v>
-      </c>
-      <c r="D14">
-        <v>0</v>
-      </c>
-      <c r="E14" s="4">
-        <v>0</v>
-      </c>
-      <c r="F14" s="10">
-        <v>0</v>
-      </c>
-      <c r="G14" s="10"/>
-      <c r="H14" s="7"/>
-      <c r="I14" s="7"/>
-      <c r="J14" s="4"/>
-      <c r="K14">
-        <v>-1000</v>
-      </c>
-      <c r="L14" s="4">
-        <v>1200000</v>
-      </c>
-      <c r="M14">
-        <v>0</v>
-      </c>
-      <c r="N14" s="4">
-        <v>0</v>
-      </c>
-      <c r="O14" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B15">
-        <v>1000</v>
-      </c>
-      <c r="C15" s="4">
-        <v>1200000</v>
-      </c>
-      <c r="D15">
-        <v>0</v>
-      </c>
-      <c r="E15" s="4">
-        <v>0</v>
-      </c>
-      <c r="F15" s="10">
-        <v>0</v>
-      </c>
-      <c r="G15" s="10"/>
-      <c r="H15" s="7"/>
-      <c r="I15" s="7"/>
-      <c r="J15" s="4"/>
-      <c r="K15">
-        <v>1000</v>
-      </c>
-      <c r="L15" s="4">
-        <v>1200000</v>
-      </c>
-      <c r="M15">
-        <v>0</v>
-      </c>
-      <c r="N15" s="4">
-        <v>0</v>
-      </c>
-      <c r="O15" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B16">
-        <v>-10000</v>
-      </c>
-      <c r="C16" s="4">
-        <v>1200000</v>
-      </c>
-      <c r="D16">
-        <v>0</v>
-      </c>
-      <c r="E16" s="4">
-        <v>0</v>
-      </c>
-      <c r="F16" s="10">
-        <v>0</v>
-      </c>
-      <c r="G16" s="10"/>
-      <c r="H16" s="7"/>
-      <c r="I16" s="7"/>
-      <c r="J16" s="4"/>
-      <c r="K16">
-        <v>-10000</v>
-      </c>
-      <c r="L16" s="4">
-        <v>1200000</v>
-      </c>
-      <c r="M16">
-        <v>0</v>
-      </c>
-      <c r="N16" s="4">
-        <v>0</v>
-      </c>
-      <c r="O16" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B17">
-        <v>10000</v>
-      </c>
-      <c r="C17" s="4">
-        <v>1200000</v>
-      </c>
-      <c r="D17">
-        <v>0</v>
-      </c>
-      <c r="E17" s="4">
-        <v>0</v>
-      </c>
-      <c r="F17" s="10">
-        <v>0</v>
-      </c>
-      <c r="G17" s="10"/>
-      <c r="H17" s="7"/>
-      <c r="I17" s="7"/>
-      <c r="J17" s="4"/>
-      <c r="K17">
-        <v>10000</v>
-      </c>
-      <c r="L17" s="4">
-        <v>1200000</v>
-      </c>
-      <c r="M17">
-        <v>0</v>
-      </c>
-      <c r="N17" s="4">
-        <v>0</v>
-      </c>
-      <c r="O17" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B18">
-        <v>0</v>
-      </c>
-      <c r="C18" s="4">
-        <v>1200000</v>
-      </c>
-      <c r="D18">
-        <v>0</v>
-      </c>
-      <c r="E18" s="4">
-        <v>0</v>
-      </c>
-      <c r="F18" s="10">
-        <v>0</v>
-      </c>
-      <c r="G18" s="10"/>
-      <c r="H18" s="7"/>
-      <c r="I18" s="7"/>
-      <c r="J18" s="4"/>
-      <c r="K18">
-        <v>0</v>
-      </c>
-      <c r="L18" s="4">
-        <v>1200000</v>
-      </c>
-      <c r="M18">
-        <v>0</v>
-      </c>
-      <c r="N18" s="4">
-        <v>0</v>
-      </c>
-      <c r="O18" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B19">
-        <v>-100</v>
-      </c>
-      <c r="C19" s="4">
-        <v>1200000</v>
-      </c>
-      <c r="D19">
-        <v>0</v>
-      </c>
-      <c r="E19" s="4">
-        <v>0</v>
-      </c>
-      <c r="F19" s="10">
-        <v>0</v>
-      </c>
-      <c r="G19" s="10"/>
-      <c r="H19" s="7"/>
-      <c r="I19" s="7"/>
-      <c r="J19" s="4"/>
-      <c r="K19">
-        <v>-100</v>
-      </c>
-      <c r="L19" s="4">
-        <v>1200000</v>
-      </c>
-      <c r="M19">
-        <v>0</v>
-      </c>
-      <c r="N19" s="4">
-        <v>0</v>
-      </c>
-      <c r="O19" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B20">
+      <c r="E29" s="4">
+        <v>0</v>
+      </c>
+      <c r="F29" s="10">
+        <v>0</v>
+      </c>
+      <c r="G29" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="H29" s="10"/>
+      <c r="K29" s="4"/>
+      <c r="M29" s="4">
+        <v>1200000</v>
+      </c>
+      <c r="O29" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="B30">
+        <v>0</v>
+      </c>
+      <c r="C30" s="19">
+        <v>1200000</v>
+      </c>
+      <c r="D30">
+        <v>0</v>
+      </c>
+      <c r="E30" s="4">
         <v>100</v>
       </c>
-      <c r="C20" s="4">
-        <v>1200000</v>
-      </c>
-      <c r="D20">
-        <v>0</v>
-      </c>
-      <c r="E20" s="4">
-        <v>0</v>
-      </c>
-      <c r="F20" s="10">
-        <v>0</v>
-      </c>
-      <c r="G20" s="10"/>
-      <c r="H20" s="7"/>
-      <c r="I20" s="7"/>
-      <c r="J20" s="4"/>
-      <c r="K20">
-        <v>100</v>
-      </c>
-      <c r="L20" s="4">
-        <v>1200000</v>
-      </c>
-      <c r="M20">
-        <v>0</v>
-      </c>
-      <c r="N20" s="4">
-        <v>0</v>
-      </c>
-      <c r="O20" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B21">
-        <v>-1000</v>
-      </c>
-      <c r="C21" s="4">
-        <v>1200000</v>
-      </c>
-      <c r="D21">
-        <v>0</v>
-      </c>
-      <c r="E21" s="4">
-        <v>0</v>
-      </c>
-      <c r="F21" s="10">
-        <v>0</v>
-      </c>
-      <c r="G21" s="10"/>
-      <c r="H21" s="7"/>
-      <c r="I21" s="7"/>
-      <c r="J21" s="4"/>
-      <c r="K21">
-        <v>-1000</v>
-      </c>
-      <c r="L21" s="4">
-        <v>1200000</v>
-      </c>
-      <c r="M21">
-        <v>0</v>
-      </c>
-      <c r="N21" s="4">
-        <v>0</v>
-      </c>
-      <c r="O21" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B22">
-        <v>1000</v>
-      </c>
-      <c r="C22" s="4">
-        <v>1200000</v>
-      </c>
-      <c r="D22">
-        <v>0</v>
-      </c>
-      <c r="E22" s="4">
-        <v>0</v>
-      </c>
-      <c r="F22" s="10">
-        <v>0</v>
-      </c>
-      <c r="G22" s="10"/>
-      <c r="H22" s="7"/>
-      <c r="I22" s="7"/>
-      <c r="J22" s="4"/>
-      <c r="K22">
-        <v>1000</v>
-      </c>
-      <c r="L22" s="4">
-        <v>1200000</v>
-      </c>
-      <c r="M22">
-        <v>0</v>
-      </c>
-      <c r="N22" s="4">
-        <v>0</v>
-      </c>
-      <c r="O22" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B23">
-        <v>-10000</v>
-      </c>
-      <c r="C23" s="4">
-        <v>1200000</v>
-      </c>
-      <c r="D23">
-        <v>0</v>
-      </c>
-      <c r="E23" s="4">
-        <v>0</v>
-      </c>
-      <c r="F23" s="10">
-        <v>0</v>
-      </c>
-      <c r="G23" s="10"/>
-      <c r="H23" s="7"/>
-      <c r="I23" s="7"/>
-      <c r="J23" s="4"/>
-      <c r="K23">
-        <v>-10000</v>
-      </c>
-      <c r="L23" s="4">
-        <v>1200000</v>
-      </c>
-      <c r="M23">
-        <v>0</v>
-      </c>
-      <c r="N23" s="4">
-        <v>0</v>
-      </c>
-      <c r="O23" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B24">
-        <v>10000</v>
-      </c>
-      <c r="C24" s="4">
-        <v>1200000</v>
-      </c>
-      <c r="D24">
-        <v>0</v>
-      </c>
-      <c r="E24" s="4">
-        <v>0</v>
-      </c>
-      <c r="F24" s="10">
-        <v>0</v>
-      </c>
-      <c r="G24" s="10"/>
-      <c r="H24" s="7"/>
-      <c r="I24" s="7"/>
-      <c r="J24" s="4"/>
-      <c r="K24">
-        <v>10000</v>
-      </c>
-      <c r="L24" s="4">
-        <v>1200000</v>
-      </c>
-      <c r="M24">
-        <v>0</v>
-      </c>
-      <c r="N24" s="4">
-        <v>0</v>
-      </c>
-      <c r="O24" s="10">
+      <c r="F30" s="10">
+        <v>0</v>
+      </c>
+      <c r="G30" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="H30" s="10"/>
+      <c r="K30" s="4"/>
+      <c r="M30" s="4">
+        <v>1200000</v>
+      </c>
+      <c r="O30" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="B31">
+        <v>0</v>
+      </c>
+      <c r="C31" s="19">
+        <v>1200000</v>
+      </c>
+      <c r="D31">
+        <v>0</v>
+      </c>
+      <c r="E31" s="19">
+        <v>0</v>
+      </c>
+      <c r="F31">
+        <v>30</v>
+      </c>
+      <c r="G31" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="H31" s="10"/>
+      <c r="K31" s="4"/>
+      <c r="M31" s="4">
+        <v>1200000</v>
+      </c>
+      <c r="O31" s="4">
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="G2:J2"/>
+    <mergeCell ref="H2:K2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added customisation of the maxWindStrength and thruster force
</commit_message>
<xml_diff>
--- a/documentation/Phase 2 experiments/Experiments.xlsx
+++ b/documentation/Phase 2 experiments/Experiments.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\V\Documents\School\Project 2\Github\documentation\Phase 2 experiments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3B604B57-05B1-4DC7-B33C-1511056D5E58}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{232DB9D3-AA95-4C40-8F39-E31CA8D1521D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3468" yWindow="0" windowWidth="17280" windowHeight="8964" xr2:uid="{715DD086-ACD7-4858-9E34-CEA6F756B20B}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{715DD086-ACD7-4858-9E34-CEA6F756B20B}"/>
   </bookViews>
   <sheets>
     <sheet name="Open Loop" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="29">
   <si>
     <t>x</t>
   </si>
@@ -108,13 +108,16 @@
     <t>wind</t>
   </si>
   <si>
-    <t>Yes</t>
-  </si>
-  <si>
     <t>Different velocities</t>
   </si>
   <si>
     <t>Different altitudes</t>
+  </si>
+  <si>
+    <t>thrusterForce</t>
+  </si>
+  <si>
+    <t>max wind Force</t>
   </si>
 </sst>
 </file>
@@ -229,7 +232,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -258,6 +261,8 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -267,8 +272,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -585,8 +590,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCCFA795-07D1-4DA6-81B9-DD5CB576DC0E}">
   <dimension ref="B2:T55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N18" sqref="N18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -607,12 +612,12 @@
         <v>7</v>
       </c>
       <c r="G2" s="4"/>
-      <c r="H2" s="21" t="s">
+      <c r="H2" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="I2" s="20"/>
-      <c r="J2" s="20"/>
-      <c r="K2" s="22"/>
+      <c r="I2" s="22"/>
+      <c r="J2" s="22"/>
+      <c r="K2" s="24"/>
       <c r="L2" s="6" t="s">
         <v>12</v>
       </c>
@@ -661,8 +666,8 @@
       </c>
     </row>
     <row r="4" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B4" s="23" t="s">
-        <v>26</v>
+      <c r="B4" s="20" t="s">
+        <v>25</v>
       </c>
       <c r="D4">
         <v>0</v>
@@ -902,8 +907,8 @@
       <c r="Q9" s="7"/>
     </row>
     <row r="10" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B10" s="23" t="s">
-        <v>27</v>
+      <c r="B10" s="20" t="s">
+        <v>26</v>
       </c>
       <c r="D10">
         <v>0</v>
@@ -917,7 +922,7 @@
       <c r="G10" s="4">
         <v>0</v>
       </c>
-      <c r="H10" s="24">
+      <c r="H10" s="21">
         <v>179</v>
       </c>
       <c r="I10" s="2">
@@ -1250,10 +1255,10 @@
       <c r="F33" s="16"/>
       <c r="G33" s="7"/>
       <c r="H33" s="17"/>
-      <c r="I33" s="20"/>
-      <c r="J33" s="20"/>
-      <c r="K33" s="20"/>
-      <c r="L33" s="20"/>
+      <c r="I33" s="22"/>
+      <c r="J33" s="22"/>
+      <c r="K33" s="22"/>
+      <c r="L33" s="22"/>
       <c r="M33" s="16"/>
       <c r="N33" s="7"/>
       <c r="O33" s="16"/>
@@ -1624,1232 +1629,1216 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F51CB71-A509-4AC5-AC8E-6056CE32F9C4}">
-  <dimension ref="A2:P31"/>
+  <dimension ref="A1:Q32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="16.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="5" width="11.21875" customWidth="1"/>
-    <col min="6" max="7" width="13.5546875" customWidth="1"/>
-    <col min="12" max="15" width="11.21875" customWidth="1"/>
-    <col min="16" max="16" width="13.5546875" customWidth="1"/>
+    <col min="2" max="2" width="16.88671875" customWidth="1"/>
+    <col min="3" max="6" width="11.21875" customWidth="1"/>
+    <col min="7" max="8" width="13.5546875" customWidth="1"/>
+    <col min="13" max="16" width="11.21875" customWidth="1"/>
+    <col min="17" max="17" width="13.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="B2" s="6" t="s">
+    <row r="1" spans="1:17" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="C2" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="4"/>
+      <c r="E2" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="4"/>
-      <c r="F2" s="12" t="s">
+      <c r="F2" s="4"/>
+      <c r="G2" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="12" t="s">
+      <c r="H2" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="H2" s="21" t="s">
+      <c r="I2" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="I2" s="20"/>
-      <c r="J2" s="20"/>
+      <c r="J2" s="22"/>
       <c r="K2" s="22"/>
-      <c r="L2" s="6" t="s">
+      <c r="L2" s="24"/>
+      <c r="M2" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="M2" s="4"/>
-      <c r="N2" s="6" t="s">
+      <c r="N2" s="4"/>
+      <c r="O2" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="O2" s="4"/>
-      <c r="P2" s="12" t="s">
+      <c r="P2" s="4"/>
+      <c r="Q2" s="12" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="B3" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="5" t="s">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="C3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E3" s="5" t="s">
+      <c r="E3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F3" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="F3" s="15" t="s">
+      <c r="G3" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="G3" s="15"/>
-      <c r="H3" s="8" t="s">
+      <c r="H3" s="15"/>
+      <c r="I3" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="I3" s="3" t="s">
+      <c r="J3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="J3" s="3" t="s">
+      <c r="K3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="K3" s="9" t="s">
+      <c r="L3" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="L3" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="M3" s="5" t="s">
+      <c r="M3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="N3" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="N3" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="O3" s="5" t="s">
+      <c r="O3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="P3" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="P3" s="15" t="s">
+      <c r="Q3" s="15" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="B4">
-        <v>0</v>
-      </c>
-      <c r="C4" s="4">
-        <v>1200000</v>
-      </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-      <c r="E4" s="4">
-        <v>0</v>
-      </c>
-      <c r="F4" s="10">
-        <v>0</v>
-      </c>
-      <c r="G4" s="10" t="s">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4" s="4">
+        <v>1200000</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4" s="4">
+        <v>0</v>
+      </c>
+      <c r="G4" s="10">
+        <v>0</v>
+      </c>
+      <c r="H4" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="H4" s="10">
+      <c r="I4" s="10">
         <v>2</v>
       </c>
-      <c r="I4" s="2">
+      <c r="J4" s="2">
         <v>15</v>
       </c>
-      <c r="J4" s="2">
+      <c r="K4" s="2">
         <v>33</v>
       </c>
-      <c r="K4" s="11">
+      <c r="L4" s="11">
         <v>4</v>
       </c>
-      <c r="L4">
-        <v>0</v>
-      </c>
-      <c r="M4" s="4">
+      <c r="M4">
+        <v>0</v>
+      </c>
+      <c r="N4" s="4">
         <v>-0.10100000000000001</v>
       </c>
-      <c r="N4">
-        <v>0</v>
-      </c>
-      <c r="O4" s="4">
+      <c r="O4">
+        <v>0</v>
+      </c>
+      <c r="P4" s="4">
         <v>-0.94499999999999995</v>
       </c>
-      <c r="P4" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q4" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>20</v>
       </c>
-      <c r="B5">
+      <c r="C5">
         <v>-100</v>
       </c>
-      <c r="C5" s="4">
-        <v>1200000</v>
-      </c>
-      <c r="D5">
-        <v>0</v>
-      </c>
-      <c r="E5" s="4">
-        <v>0</v>
-      </c>
-      <c r="F5" s="10">
-        <v>0</v>
-      </c>
-      <c r="G5" s="10" t="s">
+      <c r="D5" s="4">
+        <v>1200000</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5" s="4">
+        <v>0</v>
+      </c>
+      <c r="G5" s="10">
+        <v>0</v>
+      </c>
+      <c r="H5" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="H5" s="10">
+      <c r="I5" s="10">
         <v>2</v>
       </c>
-      <c r="I5" s="2">
+      <c r="J5" s="2">
         <v>15</v>
       </c>
-      <c r="J5" s="2">
+      <c r="K5" s="2">
         <v>30</v>
       </c>
-      <c r="K5" s="4">
+      <c r="L5" s="4">
         <v>19</v>
       </c>
-      <c r="L5">
+      <c r="M5">
         <v>3.25</v>
       </c>
-      <c r="M5" s="4">
+      <c r="N5" s="4">
         <v>-1.635</v>
       </c>
-      <c r="N5">
+      <c r="O5">
         <v>-0.55700000000000005</v>
       </c>
-      <c r="O5" s="4">
+      <c r="P5" s="4">
         <v>-1.4159999999999999</v>
       </c>
-      <c r="P5" s="10">
+      <c r="Q5" s="10">
         <v>-2</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="B6">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="C6">
         <v>100</v>
       </c>
-      <c r="C6" s="4">
-        <v>1200000</v>
-      </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
-      <c r="E6" s="4">
-        <v>0</v>
-      </c>
-      <c r="F6" s="10">
-        <v>0</v>
-      </c>
-      <c r="G6" s="10" t="s">
+      <c r="D6" s="4">
+        <v>1200000</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6" s="4">
+        <v>0</v>
+      </c>
+      <c r="G6" s="10">
+        <v>0</v>
+      </c>
+      <c r="H6" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="H6" s="10">
+      <c r="I6" s="10">
         <v>2</v>
       </c>
-      <c r="I6" s="2">
+      <c r="J6" s="2">
         <v>15</v>
       </c>
-      <c r="J6" s="2">
+      <c r="K6" s="2">
         <v>30</v>
       </c>
-      <c r="K6" s="4">
+      <c r="L6" s="4">
         <v>1</v>
       </c>
-      <c r="L6">
+      <c r="M6">
         <v>4.8440000000000003</v>
       </c>
-      <c r="M6" s="4">
+      <c r="N6" s="4">
         <v>-3.73E-2</v>
       </c>
-      <c r="N6">
+      <c r="O6">
         <v>0.9</v>
       </c>
-      <c r="O6" s="4">
+      <c r="P6" s="4">
         <v>-0.93600000000000005</v>
       </c>
-      <c r="P6" s="10">
+      <c r="Q6" s="10">
         <v>-3</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="B7">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="C7">
         <v>-1000</v>
       </c>
-      <c r="C7" s="4">
-        <v>1200000</v>
-      </c>
-      <c r="D7">
-        <v>0</v>
-      </c>
-      <c r="E7" s="4">
-        <v>0</v>
-      </c>
-      <c r="F7" s="10">
-        <v>0</v>
-      </c>
-      <c r="G7" s="10" t="s">
+      <c r="D7" s="4">
+        <v>1200000</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7" s="4">
+        <v>0</v>
+      </c>
+      <c r="G7" s="10">
+        <v>0</v>
+      </c>
+      <c r="H7" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="H7" s="10">
+      <c r="I7" s="10">
         <v>2</v>
       </c>
-      <c r="I7" s="2">
+      <c r="J7" s="2">
         <v>15</v>
       </c>
-      <c r="J7" s="2">
+      <c r="K7" s="2">
         <v>30</v>
       </c>
-      <c r="K7" s="4">
+      <c r="L7" s="4">
         <v>17</v>
       </c>
-      <c r="L7">
+      <c r="M7">
         <v>-3.8479999999999999</v>
       </c>
-      <c r="M7" s="4">
+      <c r="N7" s="4">
         <v>-0.26600000000000001</v>
       </c>
-      <c r="N7">
+      <c r="O7">
         <v>0.71799999999999997</v>
       </c>
-      <c r="O7" s="4">
+      <c r="P7" s="4">
         <v>-1.0609999999999999</v>
       </c>
-      <c r="P7" s="10">
+      <c r="Q7" s="10">
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="B8">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="C8">
         <v>1000</v>
       </c>
-      <c r="C8" s="4">
-        <v>1200000</v>
-      </c>
-      <c r="D8">
-        <v>0</v>
-      </c>
-      <c r="E8" s="4">
-        <v>0</v>
-      </c>
-      <c r="F8" s="10">
-        <v>0</v>
-      </c>
-      <c r="G8" s="10" t="s">
+      <c r="D8" s="4">
+        <v>1200000</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8" s="4">
+        <v>0</v>
+      </c>
+      <c r="G8" s="10">
+        <v>0</v>
+      </c>
+      <c r="H8" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="H8" s="10">
+      <c r="I8" s="10">
         <v>2</v>
       </c>
-      <c r="I8" s="2">
+      <c r="J8" s="2">
         <v>15</v>
       </c>
-      <c r="J8" s="2">
+      <c r="K8" s="2">
         <v>30</v>
       </c>
-      <c r="K8" s="4">
+      <c r="L8" s="4">
         <v>9</v>
       </c>
-      <c r="L8" s="2">
+      <c r="M8" s="2">
         <v>9.6739999999999995</v>
       </c>
-      <c r="M8" s="4">
+      <c r="N8" s="4">
         <v>-0.20300000000000001</v>
       </c>
-      <c r="N8">
+      <c r="O8">
         <v>-0.81299999999999994</v>
       </c>
-      <c r="O8" s="4">
+      <c r="P8" s="4">
         <v>-1.18</v>
       </c>
-      <c r="P8" s="10">
+      <c r="Q8" s="10">
         <v>-7</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="B9">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="C9">
         <v>-10000</v>
       </c>
-      <c r="C9" s="4">
-        <v>1200000</v>
-      </c>
-      <c r="D9">
-        <v>0</v>
-      </c>
-      <c r="E9" s="4">
-        <v>0</v>
-      </c>
-      <c r="F9" s="10">
-        <v>0</v>
-      </c>
-      <c r="G9" s="10" t="s">
+      <c r="D9" s="4">
+        <v>1200000</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9" s="4">
+        <v>0</v>
+      </c>
+      <c r="G9" s="10">
+        <v>0</v>
+      </c>
+      <c r="H9" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="H9" s="10">
+      <c r="I9" s="10">
         <v>2</v>
       </c>
-      <c r="I9" s="2">
+      <c r="J9" s="2">
         <v>15</v>
       </c>
-      <c r="J9" s="2">
+      <c r="K9" s="2">
         <v>29</v>
       </c>
-      <c r="K9" s="4">
+      <c r="L9" s="4">
         <v>29</v>
       </c>
-      <c r="L9">
+      <c r="M9">
         <v>8.2430000000000003</v>
       </c>
-      <c r="M9" s="4">
+      <c r="N9" s="4">
         <v>-4.6399999999999997E-2</v>
       </c>
-      <c r="N9">
+      <c r="O9">
         <v>-0.66100000000000003</v>
       </c>
-      <c r="O9" s="4">
+      <c r="P9" s="4">
         <v>-0.52500000000000002</v>
       </c>
-      <c r="P9" s="10">
+      <c r="Q9" s="10">
         <v>-6</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="B10">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="C10">
         <v>10000</v>
       </c>
-      <c r="C10" s="4">
-        <v>1200000</v>
-      </c>
-      <c r="D10">
-        <v>0</v>
-      </c>
-      <c r="E10" s="4">
-        <v>0</v>
-      </c>
-      <c r="F10" s="10">
-        <v>0</v>
-      </c>
-      <c r="G10" s="10" t="s">
+      <c r="D10" s="4">
+        <v>1200000</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10" s="4">
+        <v>0</v>
+      </c>
+      <c r="G10" s="10">
+        <v>0</v>
+      </c>
+      <c r="H10" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="H10" s="10">
+      <c r="I10" s="10">
         <v>2</v>
       </c>
-      <c r="I10" s="2">
+      <c r="J10" s="2">
         <v>15</v>
       </c>
-      <c r="J10" s="2">
+      <c r="K10" s="2">
         <v>29</v>
       </c>
-      <c r="K10" s="4">
+      <c r="L10" s="4">
         <v>58</v>
       </c>
-      <c r="L10">
+      <c r="M10">
         <v>3.0379999999999998</v>
       </c>
-      <c r="M10" s="4">
+      <c r="N10" s="4">
         <v>-0.70399999999999996</v>
       </c>
-      <c r="N10">
+      <c r="O10">
         <v>-1.0529999999999999</v>
       </c>
-      <c r="O10" s="4">
+      <c r="P10" s="4">
         <v>-0.98499999999999999</v>
       </c>
-      <c r="P10" s="10">
+      <c r="Q10" s="10">
         <v>-4</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>21</v>
       </c>
-      <c r="B11">
-        <v>0</v>
-      </c>
-      <c r="C11" s="4">
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11" s="4">
         <v>12000</v>
       </c>
-      <c r="D11">
-        <v>0</v>
-      </c>
-      <c r="E11" s="4">
-        <v>0</v>
-      </c>
-      <c r="F11" s="10">
-        <v>0</v>
-      </c>
-      <c r="G11" s="10" t="s">
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11" s="4">
+        <v>0</v>
+      </c>
+      <c r="G11" s="10">
+        <v>0</v>
+      </c>
+      <c r="H11" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="H11" s="10"/>
-      <c r="I11" s="7"/>
+      <c r="I11" s="10"/>
       <c r="J11" s="7"/>
-      <c r="K11" s="4"/>
-      <c r="L11">
+      <c r="K11" s="7"/>
+      <c r="L11" s="4"/>
+      <c r="M11">
         <v>1000</v>
       </c>
-      <c r="M11" s="4">
-        <v>1200000</v>
-      </c>
-      <c r="N11">
-        <v>0</v>
-      </c>
-      <c r="O11" s="4">
-        <v>0</v>
-      </c>
-      <c r="P11" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="B12">
-        <v>0</v>
-      </c>
-      <c r="C12" s="4">
+      <c r="N11" s="4">
+        <v>1200000</v>
+      </c>
+      <c r="O11">
+        <v>0</v>
+      </c>
+      <c r="P11" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q11" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12" s="4">
         <v>120000</v>
       </c>
-      <c r="D12">
-        <v>0</v>
-      </c>
-      <c r="E12" s="4">
-        <v>0</v>
-      </c>
-      <c r="F12" s="10">
-        <v>0</v>
-      </c>
-      <c r="G12" s="10" t="s">
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12" s="4">
+        <v>0</v>
+      </c>
+      <c r="G12" s="10">
+        <v>0</v>
+      </c>
+      <c r="H12" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="H12" s="10"/>
-      <c r="I12" s="7"/>
+      <c r="I12" s="10"/>
       <c r="J12" s="7"/>
-      <c r="K12" s="4"/>
-      <c r="L12">
+      <c r="K12" s="7"/>
+      <c r="L12" s="4"/>
+      <c r="M12">
         <v>-10000</v>
       </c>
-      <c r="M12" s="4">
-        <v>1200000</v>
-      </c>
-      <c r="N12">
-        <v>0</v>
-      </c>
-      <c r="O12" s="4">
-        <v>0</v>
-      </c>
-      <c r="P12" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="B13">
-        <v>0</v>
-      </c>
-      <c r="C13" s="19">
-        <v>1200000</v>
-      </c>
-      <c r="D13">
-        <v>0</v>
-      </c>
-      <c r="E13" s="4">
-        <v>0</v>
-      </c>
-      <c r="F13" s="10">
-        <v>0</v>
-      </c>
-      <c r="G13" s="10" t="s">
+      <c r="N12" s="4">
+        <v>1200000</v>
+      </c>
+      <c r="O12">
+        <v>0</v>
+      </c>
+      <c r="P12" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q12" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13" s="19">
+        <v>1200000</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13" s="4">
+        <v>0</v>
+      </c>
+      <c r="G13" s="10">
+        <v>0</v>
+      </c>
+      <c r="H13" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="H13" s="10">
+      <c r="I13" s="10">
         <v>2</v>
       </c>
-      <c r="I13" s="2">
+      <c r="J13" s="2">
         <v>15</v>
       </c>
-      <c r="J13" s="2">
+      <c r="K13" s="2">
         <v>33</v>
       </c>
-      <c r="K13" s="11">
+      <c r="L13" s="4">
         <v>4</v>
       </c>
-      <c r="L13">
-        <v>0</v>
-      </c>
-      <c r="M13" s="4">
+      <c r="M13">
+        <v>0</v>
+      </c>
+      <c r="N13" s="4">
         <v>-0.10100000000000001</v>
       </c>
-      <c r="N13">
-        <v>0</v>
-      </c>
-      <c r="O13" s="4">
+      <c r="O13">
+        <v>0</v>
+      </c>
+      <c r="P13" s="4">
         <v>-0.94499999999999995</v>
       </c>
-      <c r="P13" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="B14">
-        <v>0</v>
-      </c>
-      <c r="C14" s="4">
+      <c r="Q13" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14" s="4">
         <v>12000000</v>
       </c>
-      <c r="D14">
-        <v>0</v>
-      </c>
-      <c r="E14" s="4">
-        <v>0</v>
-      </c>
-      <c r="F14" s="10">
-        <v>0</v>
-      </c>
-      <c r="G14" s="10" t="s">
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14" s="4">
+        <v>0</v>
+      </c>
+      <c r="G14" s="10">
+        <v>0</v>
+      </c>
+      <c r="H14" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="H14" s="10"/>
-      <c r="I14" s="7"/>
+      <c r="I14" s="10"/>
       <c r="J14" s="7"/>
-      <c r="K14" s="4"/>
-      <c r="L14">
-        <v>0</v>
-      </c>
-      <c r="M14" s="4">
-        <v>1200000</v>
-      </c>
-      <c r="N14">
-        <v>0</v>
-      </c>
-      <c r="O14" s="4">
-        <v>0</v>
-      </c>
-      <c r="P14" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="K14" s="7"/>
+      <c r="L14" s="4"/>
+      <c r="M14">
+        <v>0</v>
+      </c>
+      <c r="N14" s="4">
+        <v>1200000</v>
+      </c>
+      <c r="O14">
+        <v>0</v>
+      </c>
+      <c r="P14" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q14" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>19</v>
       </c>
-      <c r="B15">
-        <v>0</v>
-      </c>
-      <c r="C15" s="4">
-        <v>1200000</v>
-      </c>
-      <c r="D15">
-        <v>0</v>
-      </c>
-      <c r="E15" s="4">
-        <v>0</v>
-      </c>
-      <c r="F15" s="10">
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15" s="4">
+        <v>1200000</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="F15" s="4">
+        <v>0</v>
+      </c>
+      <c r="G15" s="10">
         <v>15</v>
       </c>
-      <c r="G15" s="10" t="s">
+      <c r="H15" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="H15" s="10">
+      <c r="I15" s="10">
         <v>2</v>
       </c>
-      <c r="I15" s="2">
+      <c r="J15" s="2">
         <v>15</v>
       </c>
-      <c r="J15" s="2">
+      <c r="K15" s="2">
         <v>29</v>
       </c>
-      <c r="K15" s="4">
+      <c r="L15" s="4">
         <v>57</v>
       </c>
-      <c r="L15">
+      <c r="M15">
         <v>4.9130000000000003</v>
       </c>
-      <c r="M15" s="18">
+      <c r="N15" s="18">
         <v>-1.66</v>
       </c>
-      <c r="N15">
+      <c r="O15">
         <v>0.71499999999999997</v>
       </c>
-      <c r="O15" s="4">
+      <c r="P15" s="4">
         <v>-1.429</v>
       </c>
-      <c r="P15" s="10">
+      <c r="Q15" s="10">
         <v>-4</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="B16">
-        <v>0</v>
-      </c>
-      <c r="C16" s="4">
-        <v>1200000</v>
-      </c>
-      <c r="D16">
-        <v>0</v>
-      </c>
-      <c r="E16" s="4">
-        <v>0</v>
-      </c>
-      <c r="F16" s="10">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="D16" s="4">
+        <v>1200000</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="F16" s="4">
+        <v>0</v>
+      </c>
+      <c r="G16" s="10">
         <v>30</v>
       </c>
-      <c r="G16" s="10" t="s">
+      <c r="H16" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="H16" s="10">
+      <c r="I16" s="10">
         <v>2</v>
       </c>
-      <c r="I16" s="2">
+      <c r="J16" s="2">
         <v>15</v>
       </c>
-      <c r="J16" s="2">
+      <c r="K16" s="2">
         <v>30</v>
       </c>
-      <c r="K16" s="4">
+      <c r="L16" s="4">
         <v>17</v>
       </c>
-      <c r="L16">
+      <c r="M16">
         <v>-2.1320000000000001</v>
       </c>
-      <c r="M16" s="4">
+      <c r="N16" s="4">
         <v>-2.13E-4</v>
       </c>
-      <c r="N16">
+      <c r="O16">
         <v>-0.66900000000000004</v>
       </c>
-      <c r="O16" s="4">
+      <c r="P16" s="4">
         <v>-1.399</v>
       </c>
-      <c r="P16" s="10">
+      <c r="Q16" s="10">
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="B17">
-        <v>0</v>
-      </c>
-      <c r="C17" s="4">
-        <v>1200000</v>
-      </c>
-      <c r="D17">
-        <v>0</v>
-      </c>
-      <c r="E17" s="4">
-        <v>0</v>
-      </c>
-      <c r="F17" s="10">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17" s="4">
+        <v>1200000</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+      <c r="F17" s="4">
+        <v>0</v>
+      </c>
+      <c r="G17" s="10">
         <v>45</v>
       </c>
-      <c r="G17" s="10" t="s">
+      <c r="H17" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="H17" s="10">
+      <c r="I17" s="10">
         <v>2</v>
       </c>
-      <c r="I17" s="2">
+      <c r="J17" s="2">
         <v>15</v>
       </c>
-      <c r="J17" s="2">
+      <c r="K17" s="2">
         <v>30</v>
       </c>
-      <c r="K17" s="4">
+      <c r="L17" s="4">
         <v>2</v>
       </c>
-      <c r="L17">
+      <c r="M17">
         <v>3.1019999999999999</v>
       </c>
-      <c r="M17" s="4">
+      <c r="N17" s="4">
         <v>-0.64700000000000002</v>
       </c>
-      <c r="N17">
+      <c r="O17">
         <v>1.0329999999999999</v>
       </c>
-      <c r="O17" s="4">
+      <c r="P17" s="4">
         <v>-1.2490000000000001</v>
       </c>
-      <c r="P17" s="10">
+      <c r="Q17" s="10">
         <v>-1</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="B18">
-        <v>0</v>
-      </c>
-      <c r="C18" s="4">
-        <v>1200000</v>
-      </c>
-      <c r="D18">
-        <v>0</v>
-      </c>
-      <c r="E18" s="4">
-        <v>0</v>
-      </c>
-      <c r="F18" s="10">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="C18">
+        <v>0</v>
+      </c>
+      <c r="D18" s="4">
+        <v>1200000</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
+      <c r="F18" s="4">
+        <v>0</v>
+      </c>
+      <c r="G18" s="10">
         <v>60</v>
       </c>
-      <c r="G18" s="10" t="s">
+      <c r="H18" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="H18" s="10">
+      <c r="I18" s="10">
         <v>2</v>
       </c>
-      <c r="I18" s="2">
+      <c r="J18" s="2">
         <v>15</v>
       </c>
-      <c r="J18" s="2">
+      <c r="K18" s="2">
         <v>29</v>
       </c>
-      <c r="K18" s="4">
+      <c r="L18" s="4">
         <v>32</v>
       </c>
-      <c r="L18">
+      <c r="M18">
         <v>-9.7279999999999998</v>
       </c>
-      <c r="M18" s="4">
+      <c r="N18" s="4">
         <v>-0.53300000000000003</v>
       </c>
-      <c r="N18">
+      <c r="O18">
         <v>0.71499999999999997</v>
       </c>
-      <c r="O18" s="4">
+      <c r="P18" s="4">
         <v>-1.1040000000000001</v>
       </c>
-      <c r="P18" s="10">
+      <c r="Q18" s="10">
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>22</v>
       </c>
-      <c r="B19">
-        <v>0</v>
-      </c>
-      <c r="C19" s="4">
-        <v>1200000</v>
-      </c>
-      <c r="D19">
+      <c r="C19">
+        <v>0</v>
+      </c>
+      <c r="D19" s="4">
+        <v>1200000</v>
+      </c>
+      <c r="E19">
         <v>100</v>
       </c>
-      <c r="E19" s="4">
-        <v>0</v>
-      </c>
-      <c r="F19" s="10">
-        <v>0</v>
-      </c>
-      <c r="G19" s="10" t="s">
+      <c r="F19" s="4">
+        <v>0</v>
+      </c>
+      <c r="G19" s="10">
+        <v>0</v>
+      </c>
+      <c r="H19" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="H19" s="10"/>
-      <c r="I19" s="7"/>
+      <c r="I19" s="10"/>
       <c r="J19" s="7"/>
-      <c r="K19" s="4"/>
-      <c r="L19">
+      <c r="K19" s="7"/>
+      <c r="L19" s="4"/>
+      <c r="M19">
         <v>-100</v>
       </c>
-      <c r="M19" s="4">
-        <v>1200000</v>
-      </c>
-      <c r="N19">
-        <v>0</v>
-      </c>
-      <c r="O19" s="4">
-        <v>0</v>
-      </c>
-      <c r="P19" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="B20">
-        <v>0</v>
-      </c>
-      <c r="C20" s="4">
-        <v>1200000</v>
-      </c>
-      <c r="D20">
+      <c r="N19" s="4">
+        <v>1200000</v>
+      </c>
+      <c r="O19">
+        <v>0</v>
+      </c>
+      <c r="P19" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q19" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="C20">
+        <v>0</v>
+      </c>
+      <c r="D20" s="4">
+        <v>1200000</v>
+      </c>
+      <c r="E20">
         <v>1000</v>
       </c>
-      <c r="E20" s="4">
-        <v>0</v>
-      </c>
-      <c r="F20" s="10">
-        <v>0</v>
-      </c>
-      <c r="G20" s="10" t="s">
+      <c r="F20" s="4">
+        <v>0</v>
+      </c>
+      <c r="G20" s="10">
+        <v>0</v>
+      </c>
+      <c r="H20" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="H20" s="10"/>
-      <c r="I20" s="7"/>
+      <c r="I20" s="10"/>
       <c r="J20" s="7"/>
-      <c r="K20" s="4"/>
-      <c r="L20">
+      <c r="K20" s="7"/>
+      <c r="L20" s="4"/>
+      <c r="M20">
         <v>100</v>
       </c>
-      <c r="M20" s="4">
-        <v>1200000</v>
-      </c>
-      <c r="N20">
-        <v>0</v>
-      </c>
-      <c r="O20" s="4">
-        <v>0</v>
-      </c>
-      <c r="P20" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="B21">
-        <v>0</v>
-      </c>
-      <c r="C21" s="4">
-        <v>1200000</v>
-      </c>
-      <c r="D21">
+      <c r="N20" s="4">
+        <v>1200000</v>
+      </c>
+      <c r="O20">
+        <v>0</v>
+      </c>
+      <c r="P20" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q20" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="C21">
+        <v>0</v>
+      </c>
+      <c r="D21" s="4">
+        <v>1200000</v>
+      </c>
+      <c r="E21">
         <v>-100</v>
       </c>
-      <c r="E21" s="4">
-        <v>0</v>
-      </c>
-      <c r="F21" s="10">
-        <v>0</v>
-      </c>
-      <c r="G21" s="10" t="s">
+      <c r="F21" s="4">
+        <v>0</v>
+      </c>
+      <c r="G21" s="10">
+        <v>0</v>
+      </c>
+      <c r="H21" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="H21" s="10"/>
-      <c r="I21" s="7"/>
+      <c r="I21" s="10"/>
       <c r="J21" s="7"/>
-      <c r="K21" s="4"/>
-      <c r="L21">
+      <c r="K21" s="7"/>
+      <c r="L21" s="4"/>
+      <c r="M21">
         <v>-1000</v>
       </c>
-      <c r="M21" s="4">
-        <v>1200000</v>
-      </c>
-      <c r="N21">
-        <v>0</v>
-      </c>
-      <c r="O21" s="4">
-        <v>0</v>
-      </c>
-      <c r="P21" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="B22">
-        <v>0</v>
-      </c>
-      <c r="C22" s="4">
-        <v>1200000</v>
-      </c>
-      <c r="D22">
+      <c r="N21" s="4">
+        <v>1200000</v>
+      </c>
+      <c r="O21">
+        <v>0</v>
+      </c>
+      <c r="P21" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q21" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="C22">
+        <v>0</v>
+      </c>
+      <c r="D22" s="4">
+        <v>1200000</v>
+      </c>
+      <c r="E22">
         <v>-1000</v>
       </c>
-      <c r="E22" s="4">
-        <v>0</v>
-      </c>
-      <c r="F22" s="10">
-        <v>0</v>
-      </c>
-      <c r="G22" s="10" t="s">
+      <c r="F22" s="4">
+        <v>0</v>
+      </c>
+      <c r="G22" s="10">
+        <v>0</v>
+      </c>
+      <c r="H22" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="H22" s="10"/>
-      <c r="I22" s="7"/>
+      <c r="I22" s="10"/>
       <c r="J22" s="7"/>
-      <c r="K22" s="4"/>
-      <c r="L22">
+      <c r="K22" s="7"/>
+      <c r="L22" s="4"/>
+      <c r="M22">
         <v>1000</v>
       </c>
-      <c r="M22" s="4">
-        <v>1200000</v>
-      </c>
-      <c r="N22">
-        <v>0</v>
-      </c>
-      <c r="O22" s="4">
-        <v>0</v>
-      </c>
-      <c r="P22" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="N22" s="4">
+        <v>1200000</v>
+      </c>
+      <c r="O22">
+        <v>0</v>
+      </c>
+      <c r="P22" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q22" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>23</v>
       </c>
-      <c r="B23">
-        <v>0</v>
-      </c>
-      <c r="C23" s="4">
-        <v>1200000</v>
-      </c>
-      <c r="D23">
-        <v>0</v>
-      </c>
-      <c r="E23" s="4">
+      <c r="C23">
+        <v>0</v>
+      </c>
+      <c r="D23" s="4">
+        <v>1200000</v>
+      </c>
+      <c r="E23">
+        <v>0</v>
+      </c>
+      <c r="F23" s="4">
         <v>100</v>
       </c>
-      <c r="F23" s="10">
-        <v>0</v>
-      </c>
-      <c r="G23" s="10" t="s">
+      <c r="G23" s="10">
+        <v>0</v>
+      </c>
+      <c r="H23" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="H23" s="10"/>
-      <c r="I23" s="7"/>
+      <c r="I23" s="10"/>
       <c r="J23" s="7"/>
-      <c r="K23" s="4"/>
-      <c r="L23">
+      <c r="K23" s="7"/>
+      <c r="L23" s="4"/>
+      <c r="M23">
         <v>-10000</v>
       </c>
-      <c r="M23" s="4">
-        <v>1200000</v>
-      </c>
-      <c r="N23">
-        <v>0</v>
-      </c>
-      <c r="O23" s="4">
-        <v>0</v>
-      </c>
-      <c r="P23" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="B24">
-        <v>0</v>
-      </c>
-      <c r="C24" s="4">
-        <v>1200000</v>
-      </c>
-      <c r="D24">
-        <v>0</v>
-      </c>
-      <c r="E24" s="4">
+      <c r="N23" s="4">
+        <v>1200000</v>
+      </c>
+      <c r="O23">
+        <v>0</v>
+      </c>
+      <c r="P23" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q23" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="C24">
+        <v>0</v>
+      </c>
+      <c r="D24" s="4">
+        <v>1200000</v>
+      </c>
+      <c r="E24">
+        <v>0</v>
+      </c>
+      <c r="F24" s="4">
         <v>1000</v>
       </c>
-      <c r="F24" s="10">
-        <v>0</v>
-      </c>
-      <c r="G24" s="10" t="s">
+      <c r="G24" s="10">
+        <v>0</v>
+      </c>
+      <c r="H24" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="H24" s="10"/>
-      <c r="I24" s="7"/>
+      <c r="I24" s="10"/>
       <c r="J24" s="7"/>
-      <c r="K24" s="4"/>
-      <c r="L24">
+      <c r="K24" s="7"/>
+      <c r="L24" s="4"/>
+      <c r="M24">
         <v>10000</v>
       </c>
-      <c r="M24" s="4">
-        <v>1200000</v>
-      </c>
-      <c r="N24">
-        <v>0</v>
-      </c>
-      <c r="O24" s="4">
-        <v>0</v>
-      </c>
-      <c r="P24" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="B25">
-        <v>0</v>
-      </c>
-      <c r="C25" s="4">
-        <v>1200000</v>
-      </c>
-      <c r="D25">
-        <v>0</v>
-      </c>
-      <c r="E25" s="4">
+      <c r="N24" s="4">
+        <v>1200000</v>
+      </c>
+      <c r="O24">
+        <v>0</v>
+      </c>
+      <c r="P24" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q24" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="C25">
+        <v>0</v>
+      </c>
+      <c r="D25" s="4">
+        <v>1200000</v>
+      </c>
+      <c r="E25">
+        <v>0</v>
+      </c>
+      <c r="F25" s="4">
         <v>-100</v>
       </c>
-      <c r="F25" s="10">
-        <v>0</v>
-      </c>
-      <c r="G25" s="10" t="s">
+      <c r="G25" s="10">
+        <v>0</v>
+      </c>
+      <c r="H25" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="H25" s="10"/>
-      <c r="K25" s="4"/>
-      <c r="M25" s="4">
-        <v>1200000</v>
-      </c>
-      <c r="O25" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="B26">
-        <v>0</v>
-      </c>
-      <c r="C26" s="4">
-        <v>1200000</v>
-      </c>
-      <c r="D26">
-        <v>0</v>
-      </c>
-      <c r="E26" s="4">
+      <c r="I25" s="10"/>
+      <c r="L25" s="4"/>
+      <c r="N25" s="4">
+        <v>1200000</v>
+      </c>
+      <c r="P25" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="C26">
+        <v>0</v>
+      </c>
+      <c r="D26" s="4">
+        <v>1200000</v>
+      </c>
+      <c r="E26">
+        <v>0</v>
+      </c>
+      <c r="F26" s="4">
         <v>-1000</v>
       </c>
-      <c r="F26" s="10">
-        <v>0</v>
-      </c>
-      <c r="G26" s="10" t="s">
+      <c r="G26" s="10">
+        <v>0</v>
+      </c>
+      <c r="H26" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="H26" s="10"/>
-      <c r="K26" s="4"/>
-      <c r="M26" s="4">
-        <v>1200000</v>
-      </c>
-      <c r="O26" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
+      <c r="I26" s="10"/>
+      <c r="L26" s="4"/>
+      <c r="N26" s="4">
+        <v>1200000</v>
+      </c>
+      <c r="P26" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B27" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="H27" s="26" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
         <v>24</v>
       </c>
-      <c r="B27">
-        <v>0</v>
-      </c>
-      <c r="C27" s="4">
-        <v>1200000</v>
-      </c>
-      <c r="D27">
-        <v>0</v>
-      </c>
-      <c r="E27" s="4">
-        <v>0</v>
-      </c>
-      <c r="F27" s="10">
-        <v>0</v>
-      </c>
-      <c r="G27" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="H27" s="10"/>
-      <c r="K27" s="4"/>
-      <c r="M27" s="4">
-        <v>1200000</v>
-      </c>
-      <c r="O27" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B28">
-        <v>100</v>
-      </c>
-      <c r="C28" s="19">
-        <v>1200000</v>
-      </c>
-      <c r="D28">
-        <v>0</v>
-      </c>
-      <c r="E28" s="4">
-        <v>0</v>
-      </c>
-      <c r="F28" s="10">
-        <v>0</v>
-      </c>
-      <c r="G28" s="10" t="s">
-        <v>25</v>
+        <v>2500</v>
+      </c>
+      <c r="C28">
+        <v>0</v>
+      </c>
+      <c r="D28" s="4">
+        <v>1200000</v>
+      </c>
+      <c r="E28">
+        <v>0</v>
+      </c>
+      <c r="F28" s="4">
+        <v>0</v>
+      </c>
+      <c r="G28" s="10">
+        <v>0</v>
       </c>
       <c r="H28" s="10"/>
-      <c r="K28" s="4"/>
-      <c r="M28" s="4">
-        <v>1200000</v>
-      </c>
-      <c r="O28" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="B29">
-        <v>0</v>
-      </c>
-      <c r="C29" s="19">
-        <v>1200000</v>
-      </c>
-      <c r="D29">
-        <v>100</v>
-      </c>
-      <c r="E29" s="4">
-        <v>0</v>
-      </c>
-      <c r="F29" s="10">
-        <v>0</v>
-      </c>
-      <c r="G29" s="10" t="s">
-        <v>25</v>
+      <c r="I28" s="10"/>
+      <c r="L28" s="4"/>
+      <c r="N28" s="4"/>
+      <c r="P28" s="4"/>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="C29">
+        <v>0</v>
+      </c>
+      <c r="D29" s="19">
+        <v>1200000</v>
+      </c>
+      <c r="E29">
+        <v>0</v>
+      </c>
+      <c r="F29" s="4">
+        <v>0</v>
+      </c>
+      <c r="G29" s="10">
+        <v>0</v>
       </c>
       <c r="H29" s="10"/>
-      <c r="K29" s="4"/>
-      <c r="M29" s="4">
-        <v>1200000</v>
-      </c>
-      <c r="O29" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="B30">
-        <v>0</v>
-      </c>
-      <c r="C30" s="19">
-        <v>1200000</v>
-      </c>
-      <c r="D30">
-        <v>0</v>
-      </c>
-      <c r="E30" s="4">
-        <v>100</v>
-      </c>
-      <c r="F30" s="10">
-        <v>0</v>
-      </c>
-      <c r="G30" s="10" t="s">
-        <v>25</v>
+      <c r="I29" s="10"/>
+      <c r="L29" s="4"/>
+      <c r="N29" s="4"/>
+      <c r="P29" s="4"/>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="C30">
+        <v>0</v>
+      </c>
+      <c r="D30" s="19">
+        <v>1200000</v>
+      </c>
+      <c r="E30">
+        <v>0</v>
+      </c>
+      <c r="F30" s="4">
+        <v>0</v>
+      </c>
+      <c r="G30" s="10">
+        <v>0</v>
       </c>
       <c r="H30" s="10"/>
-      <c r="K30" s="4"/>
-      <c r="M30" s="4">
-        <v>1200000</v>
-      </c>
-      <c r="O30" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="B31">
-        <v>0</v>
-      </c>
-      <c r="C31" s="19">
-        <v>1200000</v>
-      </c>
-      <c r="D31">
-        <v>0</v>
-      </c>
-      <c r="E31" s="19">
-        <v>0</v>
-      </c>
-      <c r="F31">
-        <v>30</v>
-      </c>
-      <c r="G31" s="10" t="s">
-        <v>25</v>
+      <c r="I30" s="10"/>
+      <c r="L30" s="4"/>
+      <c r="N30" s="4"/>
+      <c r="P30" s="4"/>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="C31">
+        <v>0</v>
+      </c>
+      <c r="D31" s="19">
+        <v>1200000</v>
+      </c>
+      <c r="E31">
+        <v>0</v>
+      </c>
+      <c r="F31" s="4">
+        <v>0</v>
+      </c>
+      <c r="G31" s="10">
+        <v>0</v>
       </c>
       <c r="H31" s="10"/>
-      <c r="K31" s="4"/>
-      <c r="M31" s="4">
-        <v>1200000</v>
-      </c>
-      <c r="O31" s="4">
-        <v>0</v>
-      </c>
+      <c r="I31" s="10"/>
+      <c r="L31" s="4"/>
+      <c r="N31" s="4"/>
+      <c r="P31" s="4"/>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="C32">
+        <v>0</v>
+      </c>
+      <c r="D32" s="19">
+        <v>1200000</v>
+      </c>
+      <c r="E32">
+        <v>0</v>
+      </c>
+      <c r="F32" s="19">
+        <v>0</v>
+      </c>
+      <c r="G32">
+        <v>0</v>
+      </c>
+      <c r="H32" s="10"/>
+      <c r="I32" s="10"/>
+      <c r="L32" s="4"/>
+      <c r="N32" s="4"/>
+      <c r="P32" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="H2:K2"/>
+    <mergeCell ref="I2:L2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>